<commit_message>
New requirements.txt, updated README.md, updated excel sheets, added refined models
</commit_message>
<xml_diff>
--- a/features/refined.xlsx
+++ b/features/refined.xlsx
@@ -560,10 +560,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>6667</v>
+        <v>1999</v>
       </c>
       <c r="D4" t="n">
-        <v>3495</v>
+        <v>1086</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -573,7 +573,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.48437, -0.386  , -0.55479]), TrackedArray([0.48423, 0.41667, 1.     ]))</t>
+          <t>(TrackedArray([-0.47977, -0.37978, -0.55037]), TrackedArray([0.48001, 0.41065, 0.99418]))</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -632,10 +632,10 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>8216</v>
+        <v>1999</v>
       </c>
       <c r="D6" t="n">
-        <v>4346</v>
+        <v>1221</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -645,7 +645,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.05689,  0.43324,  0.06667]), TrackedArray([0.26034, 1.     , 0.24996]))</t>
+          <t>(TrackedArray([-0.05669,  0.43324,  0.06685]), TrackedArray([0.26011, 0.99988, 0.2491 ]))</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -668,10 +668,10 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>8773</v>
+        <v>2000</v>
       </c>
       <c r="D7" t="n">
-        <v>4710</v>
+        <v>1204</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -681,7 +681,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.50807, -0.46246, -0.67735]), TrackedArray([0.54479, 0.28949, 1.     ]))</t>
+          <t>(TrackedArray([-0.50807, -0.42704, -0.67716]), TrackedArray([0.52403, 0.28899, 0.82159]))</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -704,10 +704,10 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>17998</v>
+        <v>1999</v>
       </c>
       <c r="D8" t="n">
-        <v>9184</v>
+        <v>1129</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -717,7 +717,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.6047 , -0.84255, -0.78655]), TrackedArray([0.60478, 0.43103, 1.     ]))</t>
+          <t>(TrackedArray([-0.59729, -0.76788, -0.78242]), TrackedArray([0.59737, 0.42674, 0.99242]))</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -884,10 +884,10 @@
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>2204</v>
+        <v>2000</v>
       </c>
       <c r="D13" t="n">
-        <v>1143</v>
+        <v>1081</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -956,10 +956,10 @@
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>31432</v>
+        <v>2000</v>
       </c>
       <c r="D15" t="n">
-        <v>15752</v>
+        <v>1047</v>
       </c>
       <c r="E15" t="b">
         <v>1</v>
@@ -969,7 +969,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.21952, -1.12634, -0.77325]), TrackedArray([0.19797, 0.19003, 1.     ]))</t>
+          <t>(TrackedArray([-0.21952, -1.1262 , -0.77325]), TrackedArray([0.19438, 0.18233, 0.99894]))</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1100,10 +1100,10 @@
         <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>6052</v>
+        <v>2000</v>
       </c>
       <c r="D19" t="n">
-        <v>3051</v>
+        <v>1008</v>
       </c>
       <c r="E19" t="b">
         <v>1</v>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.22826, -0.94679, -0.81551]), TrackedArray([0.22825, 0.70258, 1.     ]))</t>
+          <t>(TrackedArray([-0.22826, -0.94679, -0.81551]), TrackedArray([0.22825, 0.70023, 0.99895]))</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1136,10 +1136,10 @@
         <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>22258</v>
+        <v>2000</v>
       </c>
       <c r="D20" t="n">
-        <v>11105</v>
+        <v>1003</v>
       </c>
       <c r="E20" t="b">
         <v>1</v>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>(TrackedArray([-1.35452, -1.22658, -0.32695]), TrackedArray([1.     , 0.95969, 0.31138]))</t>
+          <t>(TrackedArray([-1.35302, -1.22602, -0.32695]), TrackedArray([0.99634, 0.95536, 0.30617]))</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1172,10 +1172,10 @@
         <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>2568</v>
+        <v>2000</v>
       </c>
       <c r="D21" t="n">
-        <v>1288</v>
+        <v>1061</v>
       </c>
       <c r="E21" t="b">
         <v>1</v>
@@ -1244,10 +1244,10 @@
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>2442</v>
+        <v>1999</v>
       </c>
       <c r="D23" t="n">
-        <v>1238</v>
+        <v>1012</v>
       </c>
       <c r="E23" t="b">
         <v>1</v>
@@ -1280,10 +1280,10 @@
         <v>1</v>
       </c>
       <c r="C24" t="n">
-        <v>15294</v>
+        <v>1999</v>
       </c>
       <c r="D24" t="n">
-        <v>7691</v>
+        <v>1006</v>
       </c>
       <c r="E24" t="b">
         <v>1</v>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.89883, -1.2766 , -0.58423]), TrackedArray([1.     , 0.70123, 0.72898]))</t>
+          <t>(TrackedArray([-0.89268, -1.27274, -0.58278]), TrackedArray([0.99629, 0.69858, 0.72687]))</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1316,10 +1316,10 @@
         <v>10</v>
       </c>
       <c r="C25" t="n">
-        <v>26032</v>
+        <v>1999</v>
       </c>
       <c r="D25" t="n">
-        <v>19105</v>
+        <v>2228</v>
       </c>
       <c r="E25" t="b">
         <v>1</v>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.30674,  0.39881, -0.29194]), TrackedArray([0.23417, 1.     , 0.20657]))</t>
+          <t>(TrackedArray([-0.30536,  0.39881, -0.2899 ]), TrackedArray([0.23147, 0.99761, 0.20407]))</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1352,10 +1352,10 @@
         <v>10</v>
       </c>
       <c r="C26" t="n">
-        <v>16584</v>
+        <v>1999</v>
       </c>
       <c r="D26" t="n">
-        <v>11431</v>
+        <v>1683</v>
       </c>
       <c r="E26" t="b">
         <v>1</v>
@@ -1388,10 +1388,10 @@
         <v>10</v>
       </c>
       <c r="C27" t="n">
-        <v>10184</v>
+        <v>2000</v>
       </c>
       <c r="D27" t="n">
-        <v>8260</v>
+        <v>2144</v>
       </c>
       <c r="E27" t="b">
         <v>1</v>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.02419,  0.98015, -0.06189]), TrackedArray([ 0.00118,  1.     , -0.03658]))</t>
+          <t>(TrackedArray([-0.02401,  0.98015, -0.06189]), TrackedArray([ 0.00118,  1.     , -0.03658]))</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1424,10 +1424,10 @@
         <v>10</v>
       </c>
       <c r="C28" t="n">
-        <v>10544</v>
+        <v>1999</v>
       </c>
       <c r="D28" t="n">
-        <v>8453</v>
+        <v>2519</v>
       </c>
       <c r="E28" t="b">
         <v>1</v>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.74295, -4.7828 , -0.63714]), TrackedArray([ 0.89102, -3.12489,  1.     ]))</t>
+          <t>(TrackedArray([-0.71133, -4.7828 , -0.56644]), TrackedArray([ 0.81255, -3.14475,  0.93342]))</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1460,10 +1460,10 @@
         <v>10</v>
       </c>
       <c r="C29" t="n">
-        <v>17357</v>
+        <v>2000</v>
       </c>
       <c r="D29" t="n">
-        <v>13240</v>
+        <v>1965</v>
       </c>
       <c r="E29" t="b">
         <v>1</v>
@@ -1473,7 +1473,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.46804, -1.99289, -0.1205 ]), TrackedArray([ 0.77391, -1.05188,  1.     ]))</t>
+          <t>(TrackedArray([-0.46804, -1.99289, -0.12021]), TrackedArray([ 0.77391, -1.05513,  1.     ]))</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1496,10 +1496,10 @@
         <v>10</v>
       </c>
       <c r="C30" t="n">
-        <v>19610</v>
+        <v>1997</v>
       </c>
       <c r="D30" t="n">
-        <v>17830</v>
+        <v>2063</v>
       </c>
       <c r="E30" t="b">
         <v>1</v>
@@ -1532,10 +1532,10 @@
         <v>10</v>
       </c>
       <c r="C31" t="n">
-        <v>25760</v>
+        <v>2000</v>
       </c>
       <c r="D31" t="n">
-        <v>16333</v>
+        <v>2007</v>
       </c>
       <c r="E31" t="b">
         <v>1</v>
@@ -1568,10 +1568,10 @@
         <v>10</v>
       </c>
       <c r="C32" t="n">
-        <v>8864</v>
+        <v>2000</v>
       </c>
       <c r="D32" t="n">
-        <v>7930</v>
+        <v>2309</v>
       </c>
       <c r="E32" t="b">
         <v>1</v>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.03914,  0.94013,  0.06768]), TrackedArray([0.00707, 1.     , 0.11306]))</t>
+          <t>(TrackedArray([-0.03914,  0.94013,  0.06768]), TrackedArray([0.00707, 0.99883, 0.11306]))</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1604,10 +1604,10 @@
         <v>10</v>
       </c>
       <c r="C33" t="n">
-        <v>7952</v>
+        <v>2000</v>
       </c>
       <c r="D33" t="n">
-        <v>5383</v>
+        <v>1713</v>
       </c>
       <c r="E33" t="b">
         <v>1</v>
@@ -1640,10 +1640,10 @@
         <v>10</v>
       </c>
       <c r="C34" t="n">
-        <v>6764</v>
+        <v>2000</v>
       </c>
       <c r="D34" t="n">
-        <v>5331</v>
+        <v>2034</v>
       </c>
       <c r="E34" t="b">
         <v>1</v>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.1019 ,  0.70567, -0.11137]), TrackedArray([0.08881, 1.     , 0.07948]))</t>
+          <t>(TrackedArray([-0.09056,  0.70567, -0.11065]), TrackedArray([0.08652, 1.     , 0.07948]))</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -1676,10 +1676,10 @@
         <v>10</v>
       </c>
       <c r="C35" t="n">
-        <v>7196</v>
+        <v>2000</v>
       </c>
       <c r="D35" t="n">
-        <v>6257</v>
+        <v>1980</v>
       </c>
       <c r="E35" t="b">
         <v>1</v>
@@ -1712,10 +1712,10 @@
         <v>10</v>
       </c>
       <c r="C36" t="n">
-        <v>10680</v>
+        <v>1999</v>
       </c>
       <c r="D36" t="n">
-        <v>7529</v>
+        <v>1678</v>
       </c>
       <c r="E36" t="b">
         <v>1</v>
@@ -1748,10 +1748,10 @@
         <v>10</v>
       </c>
       <c r="C37" t="n">
-        <v>4292</v>
+        <v>1999</v>
       </c>
       <c r="D37" t="n">
-        <v>2950</v>
+        <v>1503</v>
       </c>
       <c r="E37" t="b">
         <v>1</v>
@@ -1964,10 +1964,10 @@
         <v>11</v>
       </c>
       <c r="C43" t="n">
-        <v>3092</v>
+        <v>2000</v>
       </c>
       <c r="D43" t="n">
-        <v>1550</v>
+        <v>1004</v>
       </c>
       <c r="E43" t="b">
         <v>1</v>
@@ -2000,10 +2000,10 @@
         <v>11</v>
       </c>
       <c r="C44" t="n">
-        <v>4076</v>
+        <v>2000</v>
       </c>
       <c r="D44" t="n">
-        <v>1899</v>
+        <v>936</v>
       </c>
       <c r="E44" t="b">
         <v>1</v>
@@ -2036,10 +2036,10 @@
         <v>11</v>
       </c>
       <c r="C45" t="n">
-        <v>2199</v>
+        <v>1999</v>
       </c>
       <c r="D45" t="n">
-        <v>1116</v>
+        <v>1016</v>
       </c>
       <c r="E45" t="b">
         <v>1</v>
@@ -2072,10 +2072,10 @@
         <v>11</v>
       </c>
       <c r="C46" t="n">
-        <v>3756</v>
+        <v>2000</v>
       </c>
       <c r="D46" t="n">
-        <v>2186</v>
+        <v>1099</v>
       </c>
       <c r="E46" t="b">
         <v>1</v>
@@ -2108,10 +2108,10 @@
         <v>11</v>
       </c>
       <c r="C47" t="n">
-        <v>2891</v>
+        <v>2000</v>
       </c>
       <c r="D47" t="n">
-        <v>1490</v>
+        <v>1017</v>
       </c>
       <c r="E47" t="b">
         <v>1</v>
@@ -2288,10 +2288,10 @@
         <v>12</v>
       </c>
       <c r="C52" t="n">
-        <v>11310</v>
+        <v>2000</v>
       </c>
       <c r="D52" t="n">
-        <v>6739</v>
+        <v>1180</v>
       </c>
       <c r="E52" t="b">
         <v>1</v>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.41825,  0.14777,  0.07737]), TrackedArray([0.82205, 1.     , 0.46521]))</t>
+          <t>(TrackedArray([-0.41825,  0.14777,  0.08498]), TrackedArray([0.82205, 1.     , 0.46486]))</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -2684,10 +2684,10 @@
         <v>12</v>
       </c>
       <c r="C63" t="n">
-        <v>2513</v>
+        <v>2000</v>
       </c>
       <c r="D63" t="n">
-        <v>1173</v>
+        <v>919</v>
       </c>
       <c r="E63" t="b">
         <v>1</v>
@@ -2697,7 +2697,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>(TrackedArray([ -9.14393,  -4.18387, -31.95971]), TrackedArray([  1.     ,   0.76844, -15.9139 ]))</t>
+          <t>(TrackedArray([ -8.99631,  -4.18387, -31.95971]), TrackedArray([  0.9195 ,   0.76844, -15.9139 ]))</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
@@ -2864,10 +2864,10 @@
         <v>13</v>
       </c>
       <c r="C68" t="n">
-        <v>2094</v>
+        <v>2000</v>
       </c>
       <c r="D68" t="n">
-        <v>1066</v>
+        <v>1019</v>
       </c>
       <c r="E68" t="b">
         <v>1</v>
@@ -2900,10 +2900,10 @@
         <v>13</v>
       </c>
       <c r="C69" t="n">
-        <v>14168</v>
+        <v>2000</v>
       </c>
       <c r="D69" t="n">
-        <v>7105</v>
+        <v>1020</v>
       </c>
       <c r="E69" t="b">
         <v>1</v>
@@ -2913,7 +2913,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>(TrackedArray([-1.54926, -0.25949, -0.19065]), TrackedArray([1.     , 0.4009 , 0.18955]))</t>
+          <t>(TrackedArray([-1.54923, -0.25949, -0.19065]), TrackedArray([1.     , 0.4009 , 0.18955]))</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -2936,10 +2936,10 @@
         <v>13</v>
       </c>
       <c r="C70" t="n">
-        <v>17806</v>
+        <v>1999</v>
       </c>
       <c r="D70" t="n">
-        <v>8547</v>
+        <v>878</v>
       </c>
       <c r="E70" t="b">
         <v>1</v>
@@ -2949,7 +2949,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>(TrackedArray([-1.04014, -0.37787, -4.36387]), TrackedArray([ 1.    ,  0.4243, -1.6978]))</t>
+          <t>(TrackedArray([-1.03799, -0.37662, -4.35215]), TrackedArray([ 0.99784,  0.4243 , -1.7022 ]))</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
@@ -2958,10 +2958,10 @@
         </is>
       </c>
       <c r="I70" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J70" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -2972,10 +2972,10 @@
         <v>13</v>
       </c>
       <c r="C71" t="n">
-        <v>34708</v>
+        <v>1999</v>
       </c>
       <c r="D71" t="n">
-        <v>17766</v>
+        <v>1100</v>
       </c>
       <c r="E71" t="b">
         <v>1</v>
@@ -2985,7 +2985,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.92803, -0.32886, -1.96752]), TrackedArray([1.     , 0.49619, 0.54516]))</t>
+          <t>(TrackedArray([-0.92803, -0.3255 , -1.96752]), TrackedArray([1.     , 0.49619, 0.44077]))</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -3008,10 +3008,10 @@
         <v>13</v>
       </c>
       <c r="C72" t="n">
-        <v>116777</v>
+        <v>2000</v>
       </c>
       <c r="D72" t="n">
-        <v>58380</v>
+        <v>997</v>
       </c>
       <c r="E72" t="b">
         <v>1</v>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.77508, -0.17131, -0.81564]), TrackedArray([0.92653, 0.26115, 1.     ]))</t>
+          <t>(TrackedArray([-0.77374, -0.17131, -0.81564]), TrackedArray([0.92653, 0.26099, 1.     ]))</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
@@ -3044,10 +3044,10 @@
         <v>13</v>
       </c>
       <c r="C73" t="n">
-        <v>3460</v>
+        <v>1999</v>
       </c>
       <c r="D73" t="n">
-        <v>2046</v>
+        <v>1210</v>
       </c>
       <c r="E73" t="b">
         <v>1</v>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.70235,  0.09724, -0.16871]), TrackedArray([1.     , 0.52287, 0.95571]))</t>
+          <t>(TrackedArray([-0.70235,  0.09724, -0.16848]), TrackedArray([1.     , 0.52285, 0.95548]))</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
@@ -3080,10 +3080,10 @@
         <v>13</v>
       </c>
       <c r="C74" t="n">
-        <v>2668</v>
+        <v>2000</v>
       </c>
       <c r="D74" t="n">
-        <v>1362</v>
+        <v>1028</v>
       </c>
       <c r="E74" t="b">
         <v>1</v>
@@ -3116,10 +3116,10 @@
         <v>13</v>
       </c>
       <c r="C75" t="n">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="D75" t="n">
-        <v>1006</v>
+        <v>1002</v>
       </c>
       <c r="E75" t="b">
         <v>1</v>
@@ -3188,10 +3188,10 @@
         <v>14</v>
       </c>
       <c r="C77" t="n">
-        <v>5323</v>
+        <v>2000</v>
       </c>
       <c r="D77" t="n">
-        <v>3574</v>
+        <v>1341</v>
       </c>
       <c r="E77" t="b">
         <v>1</v>
@@ -3201,7 +3201,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>(TrackedArray([-1.00021, -3.60927, -0.30201]), TrackedArray([ 1.     , -0.46903,  0.88352]))</t>
+          <t>(TrackedArray([-1.00021, -3.60927, -0.30181]), TrackedArray([ 0.99986, -0.46903,  0.88352]))</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
@@ -3224,10 +3224,10 @@
         <v>14</v>
       </c>
       <c r="C78" t="n">
-        <v>27535</v>
+        <v>2000</v>
       </c>
       <c r="D78" t="n">
-        <v>13609</v>
+        <v>1030</v>
       </c>
       <c r="E78" t="b">
         <v>1</v>
@@ -3237,7 +3237,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.62422, -0.59061, -0.5116 ]), TrackedArray([0.62611, 1.     , 0.87069]))</t>
+          <t>(TrackedArray([-0.61364, -0.59061, -0.5116 ]), TrackedArray([0.61921, 1.     , 0.87069]))</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -3332,10 +3332,10 @@
         <v>14</v>
       </c>
       <c r="C81" t="n">
-        <v>62933</v>
+        <v>2000</v>
       </c>
       <c r="D81" t="n">
-        <v>33128</v>
+        <v>1300</v>
       </c>
       <c r="E81" t="b">
         <v>1</v>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.65663, -0.46949, -1.10675]), TrackedArray([0.65203, 0.45189, 1.     ]))</t>
+          <t>(TrackedArray([-0.65562, -0.46782, -1.10675]), TrackedArray([0.64719, 0.45022, 1.     ]))</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
@@ -3440,10 +3440,10 @@
         <v>14</v>
       </c>
       <c r="C84" t="n">
-        <v>6073</v>
+        <v>2000</v>
       </c>
       <c r="D84" t="n">
-        <v>3099</v>
+        <v>1040</v>
       </c>
       <c r="E84" t="b">
         <v>1</v>
@@ -3453,7 +3453,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.99775, -1.73796, -0.29283]), TrackedArray([1.     , 0.66532, 0.28107]))</t>
+          <t>(TrackedArray([-0.99775, -1.73796, -0.28906]), TrackedArray([1.     , 0.66532, 0.27729]))</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
@@ -3476,10 +3476,10 @@
         <v>14</v>
       </c>
       <c r="C85" t="n">
-        <v>2496</v>
+        <v>2000</v>
       </c>
       <c r="D85" t="n">
-        <v>1293</v>
+        <v>1036</v>
       </c>
       <c r="E85" t="b">
         <v>1</v>
@@ -3548,10 +3548,10 @@
         <v>14</v>
       </c>
       <c r="C87" t="n">
-        <v>9528</v>
+        <v>2000</v>
       </c>
       <c r="D87" t="n">
-        <v>5986</v>
+        <v>1378</v>
       </c>
       <c r="E87" t="b">
         <v>1</v>
@@ -3561,7 +3561,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.25664, 0.63262, 0.22425]), TrackedArray([0.69092, 1.     , 0.33364]))</t>
+          <t>(TrackedArray([0.25664, 0.63281, 0.22438]), TrackedArray([0.69092, 0.99957, 0.33269]))</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
@@ -3620,10 +3620,10 @@
         <v>14</v>
       </c>
       <c r="C89" t="n">
-        <v>6962</v>
+        <v>2000</v>
       </c>
       <c r="D89" t="n">
-        <v>4459</v>
+        <v>1365</v>
       </c>
       <c r="E89" t="b">
         <v>1</v>
@@ -3633,7 +3633,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>(TrackedArray([-2.2805 , -0.64398, -0.91659]), TrackedArray([1.     , 0.31296, 0.19046]))</t>
+          <t>(TrackedArray([-2.2805 , -0.64398, -0.91211]), TrackedArray([0.99855, 0.23174, 0.19086]))</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
@@ -3656,10 +3656,10 @@
         <v>15</v>
       </c>
       <c r="C90" t="n">
-        <v>3260</v>
+        <v>2000</v>
       </c>
       <c r="D90" t="n">
-        <v>1644</v>
+        <v>1014</v>
       </c>
       <c r="E90" t="b">
         <v>1</v>
@@ -3692,10 +3692,10 @@
         <v>15</v>
       </c>
       <c r="C91" t="n">
-        <v>47613</v>
+        <v>1999</v>
       </c>
       <c r="D91" t="n">
-        <v>23803</v>
+        <v>1071</v>
       </c>
       <c r="E91" t="b">
         <v>1</v>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.73027, -0.73625, -1.74508]), TrackedArray([0.74629, 0.42903, 1.     ]))</t>
+          <t>(TrackedArray([-0.72436, -0.7347 , -1.74553]), TrackedArray([0.73492, 0.42903, 0.99968]))</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
@@ -3728,10 +3728,10 @@
         <v>15</v>
       </c>
       <c r="C92" t="n">
-        <v>7120</v>
+        <v>1999</v>
       </c>
       <c r="D92" t="n">
-        <v>4970</v>
+        <v>1277</v>
       </c>
       <c r="E92" t="b">
         <v>1</v>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.72304, -0.03049, -0.24514]), TrackedArray([1.     , 0.29853, 0.62515]))</t>
+          <t>(TrackedArray([-0.72304, -0.03049, -0.24514]), TrackedArray([0.99834, 0.29643, 0.62515]))</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
@@ -3764,10 +3764,10 @@
         <v>15</v>
       </c>
       <c r="C93" t="n">
-        <v>50685</v>
+        <v>2000</v>
       </c>
       <c r="D93" t="n">
-        <v>24786</v>
+        <v>1115</v>
       </c>
       <c r="E93" t="b">
         <v>1</v>
@@ -3777,7 +3777,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.50279, -0.11607, -0.16307]), TrackedArray([1.     , 0.18654, 0.11688]))</t>
+          <t>(TrackedArray([-0.44096, -0.1158 , -0.16307]), TrackedArray([1.     , 0.18654, 0.11688]))</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
@@ -3800,10 +3800,10 @@
         <v>15</v>
       </c>
       <c r="C94" t="n">
-        <v>3269</v>
+        <v>1997</v>
       </c>
       <c r="D94" t="n">
-        <v>1621</v>
+        <v>1003</v>
       </c>
       <c r="E94" t="b">
         <v>1</v>
@@ -3836,10 +3836,10 @@
         <v>15</v>
       </c>
       <c r="C95" t="n">
-        <v>21007</v>
+        <v>1999</v>
       </c>
       <c r="D95" t="n">
-        <v>10969</v>
+        <v>1109</v>
       </c>
       <c r="E95" t="b">
         <v>1</v>
@@ -3849,7 +3849,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.32383, -0.08616, -0.67978]), TrackedArray([0.32388, 0.24179, 1.     ]))</t>
+          <t>(TrackedArray([-0.32315, -0.08468, -0.67978]), TrackedArray([0.3232 , 0.24168, 1.     ]))</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
@@ -3872,10 +3872,10 @@
         <v>15</v>
       </c>
       <c r="C96" t="n">
-        <v>7879</v>
+        <v>1999</v>
       </c>
       <c r="D96" t="n">
-        <v>4284</v>
+        <v>1155</v>
       </c>
       <c r="E96" t="b">
         <v>1</v>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>(TrackedArray([-1.50618, -6.58178, -2.20529]), TrackedArray([ 1.     , -2.15557, -1.03008]))</t>
+          <t>(TrackedArray([-1.50618, -6.58178, -2.20529]), TrackedArray([ 1.     , -2.15557, -1.03283]))</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -3908,10 +3908,10 @@
         <v>15</v>
       </c>
       <c r="C97" t="n">
-        <v>12769</v>
+        <v>2000</v>
       </c>
       <c r="D97" t="n">
-        <v>6514</v>
+        <v>1079</v>
       </c>
       <c r="E97" t="b">
         <v>1</v>
@@ -3921,7 +3921,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.39699, -0.12343, -0.82527]), TrackedArray([0.39603, 0.23794, 1.     ]))</t>
+          <t>(TrackedArray([-0.39699, -0.1212 , -0.82527]), TrackedArray([0.39603, 0.23794, 1.     ]))</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
@@ -3944,10 +3944,10 @@
         <v>15</v>
       </c>
       <c r="C98" t="n">
-        <v>10492</v>
+        <v>1998</v>
       </c>
       <c r="D98" t="n">
-        <v>4332</v>
+        <v>554</v>
       </c>
       <c r="E98" t="b">
         <v>1</v>
@@ -3957,7 +3957,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.98808, -0.04003, -0.61654]), TrackedArray([1.     , 0.35263, 0.20993]))</t>
+          <t>(TrackedArray([-0.98601, -0.04003, -0.6158 ]), TrackedArray([0.84523, 0.35106, 0.2092 ]))</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
@@ -3966,10 +3966,10 @@
         </is>
       </c>
       <c r="I98" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J98" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -3980,10 +3980,10 @@
         <v>15</v>
       </c>
       <c r="C99" t="n">
-        <v>95045</v>
+        <v>2000</v>
       </c>
       <c r="D99" t="n">
-        <v>47474</v>
+        <v>1046</v>
       </c>
       <c r="E99" t="b">
         <v>1</v>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.62152, -0.3298 , -1.21918]), TrackedArray([0.61087, 0.5145 , 1.     ]))</t>
+          <t>(TrackedArray([-0.62152, -0.32683, -1.21918]), TrackedArray([0.61087, 0.5145 , 0.99841]))</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
@@ -4016,10 +4016,10 @@
         <v>15</v>
       </c>
       <c r="C100" t="n">
-        <v>109357</v>
+        <v>2000</v>
       </c>
       <c r="D100" t="n">
-        <v>54710</v>
+        <v>1048</v>
       </c>
       <c r="E100" t="b">
         <v>1</v>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.45707, -0.13262, -0.86615]), TrackedArray([0.45251, 0.30019, 1.     ]))</t>
+          <t>(TrackedArray([-0.45707, -0.1318 , -0.86615]), TrackedArray([0.45251, 0.29995, 1.     ]))</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
@@ -4052,10 +4052,10 @@
         <v>15</v>
       </c>
       <c r="C101" t="n">
-        <v>20577</v>
+        <v>2000</v>
       </c>
       <c r="D101" t="n">
-        <v>10604</v>
+        <v>1038</v>
       </c>
       <c r="E101" t="b">
         <v>1</v>
@@ -4065,7 +4065,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.7296 , -0.16279, -1.48031]), TrackedArray([0.7218 , 0.42704, 1.     ]))</t>
+          <t>(TrackedArray([-0.7296 , -0.16169, -1.47266]), TrackedArray([0.7218 , 0.42704, 1.     ]))</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -4088,10 +4088,10 @@
         <v>15</v>
       </c>
       <c r="C102" t="n">
-        <v>11468</v>
+        <v>2000</v>
       </c>
       <c r="D102" t="n">
-        <v>6808</v>
+        <v>1294</v>
       </c>
       <c r="E102" t="b">
         <v>1</v>
@@ -4101,7 +4101,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>(TrackedArray([-1.16709, -0.31634, -0.09279]), TrackedArray([1.     , 0.49258, 0.41537]))</t>
+          <t>(TrackedArray([-1.16558, -0.3162 , -0.0927 ]), TrackedArray([1.     , 0.49232, 0.41241]))</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
@@ -4160,10 +4160,10 @@
         <v>16</v>
       </c>
       <c r="C104" t="n">
-        <v>13450</v>
+        <v>2000</v>
       </c>
       <c r="D104" t="n">
-        <v>6727</v>
+        <v>1002</v>
       </c>
       <c r="E104" t="b">
         <v>1</v>
@@ -4173,7 +4173,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.39758, -0.42226, -0.39744]), TrackedArray([0.39758, 1.     , 0.39574]))</t>
+          <t>(TrackedArray([-0.39736, -0.42226, -0.39674]), TrackedArray([0.39504, 1.     , 0.39552]))</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
@@ -4196,10 +4196,10 @@
         <v>16</v>
       </c>
       <c r="C105" t="n">
-        <v>3080</v>
+        <v>2000</v>
       </c>
       <c r="D105" t="n">
-        <v>1542</v>
+        <v>1002</v>
       </c>
       <c r="E105" t="b">
         <v>1</v>
@@ -4340,10 +4340,10 @@
         <v>16</v>
       </c>
       <c r="C109" t="n">
-        <v>4750</v>
+        <v>1999</v>
       </c>
       <c r="D109" t="n">
-        <v>2386</v>
+        <v>1008</v>
       </c>
       <c r="E109" t="b">
         <v>1</v>
@@ -4484,10 +4484,10 @@
         <v>16</v>
       </c>
       <c r="C113" t="n">
-        <v>12192</v>
+        <v>1999</v>
       </c>
       <c r="D113" t="n">
-        <v>6094</v>
+        <v>1004</v>
       </c>
       <c r="E113" t="b">
         <v>1</v>
@@ -4497,7 +4497,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.50224, -0.53629, -0.50199]), TrackedArray([0.50223, 1.     , 0.50197]))</t>
+          <t>(TrackedArray([-0.49801, -0.53629, -0.50059]), TrackedArray([0.50011, 0.99802, 0.5004 ]))</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
@@ -4520,10 +4520,10 @@
         <v>16</v>
       </c>
       <c r="C114" t="n">
-        <v>2944</v>
+        <v>2000</v>
       </c>
       <c r="D114" t="n">
-        <v>1474</v>
+        <v>1002</v>
       </c>
       <c r="E114" t="b">
         <v>1</v>
@@ -4556,10 +4556,10 @@
         <v>16</v>
       </c>
       <c r="C115" t="n">
-        <v>2600</v>
+        <v>2000</v>
       </c>
       <c r="D115" t="n">
-        <v>1282</v>
+        <v>994</v>
       </c>
       <c r="E115" t="b">
         <v>1</v>
@@ -4592,10 +4592,10 @@
         <v>17</v>
       </c>
       <c r="C116" t="n">
-        <v>3318</v>
+        <v>2000</v>
       </c>
       <c r="D116" t="n">
-        <v>1740</v>
+        <v>1082</v>
       </c>
       <c r="E116" t="b">
         <v>1</v>
@@ -4736,10 +4736,10 @@
         <v>17</v>
       </c>
       <c r="C120" t="n">
-        <v>7638</v>
+        <v>2000</v>
       </c>
       <c r="D120" t="n">
-        <v>3884</v>
+        <v>1134</v>
       </c>
       <c r="E120" t="b">
         <v>1</v>
@@ -5024,10 +5024,10 @@
         <v>17</v>
       </c>
       <c r="C128" t="n">
-        <v>3468</v>
+        <v>2000</v>
       </c>
       <c r="D128" t="n">
-        <v>1724</v>
+        <v>990</v>
       </c>
       <c r="E128" t="b">
         <v>1</v>
@@ -5096,10 +5096,10 @@
         <v>18</v>
       </c>
       <c r="C130" t="n">
-        <v>2046</v>
+        <v>2000</v>
       </c>
       <c r="D130" t="n">
-        <v>1146</v>
+        <v>1123</v>
       </c>
       <c r="E130" t="b">
         <v>1</v>
@@ -5240,10 +5240,10 @@
         <v>18</v>
       </c>
       <c r="C134" t="n">
-        <v>2450</v>
+        <v>1999</v>
       </c>
       <c r="D134" t="n">
-        <v>1336</v>
+        <v>1110</v>
       </c>
       <c r="E134" t="b">
         <v>1</v>
@@ -5312,10 +5312,10 @@
         <v>18</v>
       </c>
       <c r="C136" t="n">
-        <v>11832</v>
+        <v>2000</v>
       </c>
       <c r="D136" t="n">
-        <v>5930</v>
+        <v>1014</v>
       </c>
       <c r="E136" t="b">
         <v>1</v>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>(TrackedArray([-1.21139, -0.2426 , -0.78241]), TrackedArray([1.     , 0.3879 , 0.97508]))</t>
+          <t>(TrackedArray([-1.21139, -0.2426 , -0.78227]), TrackedArray([0.99999, 0.38694, 0.97508]))</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
@@ -5348,10 +5348,10 @@
         <v>18</v>
       </c>
       <c r="C137" t="n">
-        <v>7250</v>
+        <v>1999</v>
       </c>
       <c r="D137" t="n">
-        <v>3823</v>
+        <v>1012</v>
       </c>
       <c r="E137" t="b">
         <v>1</v>
@@ -5361,7 +5361,7 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.66031, -0.70769, -0.70634]), TrackedArray([0.66028, 1.     , 0.85486]))</t>
+          <t>(TrackedArray([-0.65977, -0.70769, -0.7038 ]), TrackedArray([0.66028, 0.99941, 0.85486]))</t>
         </is>
       </c>
       <c r="H137" t="inlineStr">
@@ -5384,10 +5384,10 @@
         <v>18</v>
       </c>
       <c r="C138" t="n">
-        <v>26946</v>
+        <v>2000</v>
       </c>
       <c r="D138" t="n">
-        <v>15277</v>
+        <v>1014</v>
       </c>
       <c r="E138" t="b">
         <v>1</v>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.99926, -0.28604, -0.54402]), TrackedArray([1.     , 0.59156, 0.96566]))</t>
+          <t>(TrackedArray([-0.99926, -0.28604, -0.54402]), TrackedArray([1.     , 0.58705, 0.96566]))</t>
         </is>
       </c>
       <c r="H138" t="inlineStr">
@@ -5600,10 +5600,10 @@
         <v>2</v>
       </c>
       <c r="C144" t="n">
-        <v>2547</v>
+        <v>2000</v>
       </c>
       <c r="D144" t="n">
-        <v>1350</v>
+        <v>1046</v>
       </c>
       <c r="E144" t="b">
         <v>1</v>
@@ -5636,10 +5636,10 @@
         <v>2</v>
       </c>
       <c r="C145" t="n">
-        <v>32574</v>
+        <v>2000</v>
       </c>
       <c r="D145" t="n">
-        <v>16287</v>
+        <v>1001</v>
       </c>
       <c r="E145" t="b">
         <v>1</v>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.48746, -0.17671, -0.51986]), TrackedArray([0.49313, 0.19055, 1.     ]))</t>
+          <t>(TrackedArray([-0.48541, -0.17342, -0.5191 ]), TrackedArray([0.49129, 0.18957, 0.998  ]))</t>
         </is>
       </c>
       <c r="H145" t="inlineStr">
@@ -5744,10 +5744,10 @@
         <v>2</v>
       </c>
       <c r="C148" t="n">
-        <v>2338</v>
+        <v>1997</v>
       </c>
       <c r="D148" t="n">
-        <v>1224</v>
+        <v>1027</v>
       </c>
       <c r="E148" t="b">
         <v>1</v>
@@ -5757,7 +5757,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.34203, -1.0526 , -0.18666]), TrackedArray([0.3402 , 1.     , 0.52362]))</t>
+          <t>(TrackedArray([-0.34203, -1.0521 , -0.18666]), TrackedArray([0.3402 , 1.     , 0.52362]))</t>
         </is>
       </c>
       <c r="H148" t="inlineStr">
@@ -5816,10 +5816,10 @@
         <v>2</v>
       </c>
       <c r="C150" t="n">
-        <v>6102</v>
+        <v>2000</v>
       </c>
       <c r="D150" t="n">
-        <v>3071</v>
+        <v>1105</v>
       </c>
       <c r="E150" t="b">
         <v>1</v>
@@ -5829,7 +5829,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.65736, -0.72886, -3.54295]), TrackedArray([0.58018, 0.39835, 1.     ]))</t>
+          <t>(TrackedArray([-0.65672, -0.72563, -3.54295]), TrackedArray([0.57825, 0.39835, 1.     ]))</t>
         </is>
       </c>
       <c r="H150" t="inlineStr">
@@ -5852,10 +5852,10 @@
         <v>2</v>
       </c>
       <c r="C151" t="n">
-        <v>5926</v>
+        <v>2000</v>
       </c>
       <c r="D151" t="n">
-        <v>3238</v>
+        <v>1150</v>
       </c>
       <c r="E151" t="b">
         <v>1</v>
@@ -5865,7 +5865,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.86807, -3.51277, -0.34422]), TrackedArray([0.69948, 1.     , 0.99379]))</t>
+          <t>(TrackedArray([-0.86807, -3.51277, -0.34422]), TrackedArray([0.69502, 1.     , 0.99379]))</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
@@ -5996,10 +5996,10 @@
         <v>2</v>
       </c>
       <c r="C155" t="n">
-        <v>5476</v>
+        <v>1999</v>
       </c>
       <c r="D155" t="n">
-        <v>2640</v>
+        <v>973</v>
       </c>
       <c r="E155" t="b">
         <v>1</v>
@@ -6009,7 +6009,7 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.36688, -1.20126, -0.22027]), TrackedArray([0.36294, 1.     , 0.25027]))</t>
+          <t>(TrackedArray([-0.36463, -1.20047, -0.22027]), TrackedArray([0.36294, 1.     , 0.24727]))</t>
         </is>
       </c>
       <c r="H155" t="inlineStr">
@@ -6032,10 +6032,10 @@
         <v>2</v>
       </c>
       <c r="C156" t="n">
-        <v>2576</v>
+        <v>2000</v>
       </c>
       <c r="D156" t="n">
-        <v>1290</v>
+        <v>1002</v>
       </c>
       <c r="E156" t="b">
         <v>1</v>
@@ -6045,7 +6045,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.58109, -1.10662, -0.17335]), TrackedArray([0.59728, 1.     , 0.17741]))</t>
+          <t>(TrackedArray([-0.58054, -1.10662, -0.17335]), TrackedArray([0.59612, 1.     , 0.17741]))</t>
         </is>
       </c>
       <c r="H156" t="inlineStr">
@@ -6104,10 +6104,10 @@
         <v>3</v>
       </c>
       <c r="C158" t="n">
-        <v>34333</v>
+        <v>1999</v>
       </c>
       <c r="D158" t="n">
-        <v>17526</v>
+        <v>1100</v>
       </c>
       <c r="E158" t="b">
         <v>1</v>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.04194, -0.05098,  0.56213]), TrackedArray([0.48298, 0.63257, 1.     ]))</t>
+          <t>(TrackedArray([-0.04177, -0.04693,  0.56357]), TrackedArray([0.48246, 0.62985, 0.9982 ]))</t>
         </is>
       </c>
       <c r="H158" t="inlineStr">
@@ -6140,10 +6140,10 @@
         <v>3</v>
       </c>
       <c r="C159" t="n">
-        <v>3972</v>
+        <v>2000</v>
       </c>
       <c r="D159" t="n">
-        <v>2081</v>
+        <v>1086</v>
       </c>
       <c r="E159" t="b">
         <v>1</v>
@@ -6153,7 +6153,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.51496, -0.28595, -0.6533 ]), TrackedArray([0.54143, 1.     , 0.16583]))</t>
+          <t>(TrackedArray([-0.51496, -0.28378, -0.6533 ]), TrackedArray([0.54143, 1.     , 0.16521]))</t>
         </is>
       </c>
       <c r="H159" t="inlineStr">
@@ -6176,10 +6176,10 @@
         <v>3</v>
       </c>
       <c r="C160" t="n">
-        <v>316498</v>
+        <v>2000</v>
       </c>
       <c r="D160" t="n">
-        <v>160940</v>
+        <v>1104</v>
       </c>
       <c r="E160" t="b">
         <v>1</v>
@@ -6189,7 +6189,7 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.30672,  0.08012, -0.42847]), TrackedArray([0.30581, 1.     , 0.34489]))</t>
+          <t>(TrackedArray([-0.29575,  0.08963, -0.42586]), TrackedArray([0.30322, 0.98437, 0.34246]))</t>
         </is>
       </c>
       <c r="H160" t="inlineStr">
@@ -6212,10 +6212,10 @@
         <v>3</v>
       </c>
       <c r="C161" t="n">
-        <v>37922</v>
+        <v>2000</v>
       </c>
       <c r="D161" t="n">
-        <v>19324</v>
+        <v>1104</v>
       </c>
       <c r="E161" t="b">
         <v>1</v>
@@ -6225,7 +6225,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.35312,  0.20356, -0.58154]), TrackedArray([ 0.33537,  1.     , -0.01775]))</t>
+          <t>(TrackedArray([-0.35312,  0.20374, -0.58154]), TrackedArray([ 0.33517,  1.     , -0.01938]))</t>
         </is>
       </c>
       <c r="H161" t="inlineStr">
@@ -6248,10 +6248,10 @@
         <v>3</v>
       </c>
       <c r="C162" t="n">
-        <v>2158</v>
+        <v>1999</v>
       </c>
       <c r="D162" t="n">
-        <v>1174</v>
+        <v>1054</v>
       </c>
       <c r="E162" t="b">
         <v>1</v>
@@ -6261,7 +6261,7 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.71158, -1.23527, -0.35808]), TrackedArray([0.6846 , 1.     , 0.51485]))</t>
+          <t>(TrackedArray([-0.71158, -1.23527, -0.35808]), TrackedArray([0.68395, 1.     , 0.51485]))</t>
         </is>
       </c>
       <c r="H162" t="inlineStr">
@@ -6284,10 +6284,10 @@
         <v>3</v>
       </c>
       <c r="C163" t="n">
-        <v>6226</v>
+        <v>2000</v>
       </c>
       <c r="D163" t="n">
-        <v>3390</v>
+        <v>1126</v>
       </c>
       <c r="E163" t="b">
         <v>1</v>
@@ -6297,7 +6297,7 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.5343, -0.3976, -1.087 ]), TrackedArray([0.48649, 1.     , 0.03362]))</t>
+          <t>(TrackedArray([-0.53135, -0.3976 , -1.07459]), TrackedArray([0.48649, 1.     , 0.03362]))</t>
         </is>
       </c>
       <c r="H163" t="inlineStr">
@@ -6320,10 +6320,10 @@
         <v>3</v>
       </c>
       <c r="C164" t="n">
-        <v>2955</v>
+        <v>2000</v>
       </c>
       <c r="D164" t="n">
-        <v>1581</v>
+        <v>1076</v>
       </c>
       <c r="E164" t="b">
         <v>1</v>
@@ -6356,10 +6356,10 @@
         <v>3</v>
       </c>
       <c r="C165" t="n">
-        <v>4452</v>
+        <v>2000</v>
       </c>
       <c r="D165" t="n">
-        <v>2307</v>
+        <v>1078</v>
       </c>
       <c r="E165" t="b">
         <v>1</v>
@@ -6369,7 +6369,7 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.00875,  0.2346 ,  0.24769]), TrackedArray([0.63309, 1.     , 0.74191]))</t>
+          <t>(TrackedArray([-0.00393,  0.2346 ,  0.2526 ]), TrackedArray([0.63309, 1.     , 0.74191]))</t>
         </is>
       </c>
       <c r="H165" t="inlineStr">
@@ -6392,10 +6392,10 @@
         <v>3</v>
       </c>
       <c r="C166" t="n">
-        <v>3961</v>
+        <v>2000</v>
       </c>
       <c r="D166" t="n">
-        <v>2017</v>
+        <v>1034</v>
       </c>
       <c r="E166" t="b">
         <v>1</v>
@@ -6405,7 +6405,7 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.20355, 0.34103, 0.44087]), TrackedArray([0.63256, 1.     , 0.73031]))</t>
+          <t>(TrackedArray([0.20355, 0.34103, 0.44087]), TrackedArray([0.63256, 1.     , 0.73016]))</t>
         </is>
       </c>
       <c r="H166" t="inlineStr">
@@ -6428,10 +6428,10 @@
         <v>3</v>
       </c>
       <c r="C167" t="n">
-        <v>3984</v>
+        <v>2000</v>
       </c>
       <c r="D167" t="n">
-        <v>2045</v>
+        <v>1050</v>
       </c>
       <c r="E167" t="b">
         <v>1</v>
@@ -6441,7 +6441,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.07734,  0.08201,  0.41253]), TrackedArray([0.57209, 1.     , 0.87339]))</t>
+          <t>(TrackedArray([-0.0674 ,  0.08201,  0.42294]), TrackedArray([0.57209, 1.     , 0.87338]))</t>
         </is>
       </c>
       <c r="H167" t="inlineStr">
@@ -6464,10 +6464,10 @@
         <v>3</v>
       </c>
       <c r="C168" t="n">
-        <v>6468</v>
+        <v>1999</v>
       </c>
       <c r="D168" t="n">
-        <v>3300</v>
+        <v>1059</v>
       </c>
       <c r="E168" t="b">
         <v>1</v>
@@ -6477,7 +6477,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.1753 ,  0.02568,  0.50922]), TrackedArray([0.51023, 1.     , 0.8926 ]))</t>
+          <t>(TrackedArray([-0.1753 ,  0.02568,  0.50922]), TrackedArray([0.51023, 1.     , 0.89234]))</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
@@ -6500,10 +6500,10 @@
         <v>3</v>
       </c>
       <c r="C169" t="n">
-        <v>4052</v>
+        <v>1999</v>
       </c>
       <c r="D169" t="n">
-        <v>2085</v>
+        <v>1056</v>
       </c>
       <c r="E169" t="b">
         <v>1</v>
@@ -6572,10 +6572,10 @@
         <v>4</v>
       </c>
       <c r="C171" t="n">
-        <v>13373</v>
+        <v>1999</v>
       </c>
       <c r="D171" t="n">
-        <v>6918</v>
+        <v>1162</v>
       </c>
       <c r="E171" t="b">
         <v>1</v>
@@ -6608,10 +6608,10 @@
         <v>4</v>
       </c>
       <c r="C172" t="n">
-        <v>41681</v>
+        <v>2000</v>
       </c>
       <c r="D172" t="n">
-        <v>21085</v>
+        <v>1099</v>
       </c>
       <c r="E172" t="b">
         <v>1</v>
@@ -6621,7 +6621,7 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.43079, -0.3684 , -0.43979]), TrackedArray([0.46952, 1.     , 0.48284]))</t>
+          <t>(TrackedArray([-0.43079, -0.3684 , -0.43979]), TrackedArray([0.46952, 0.96629, 0.48284]))</t>
         </is>
       </c>
       <c r="H172" t="inlineStr">
@@ -6644,10 +6644,10 @@
         <v>4</v>
       </c>
       <c r="C173" t="n">
-        <v>89968</v>
+        <v>2000</v>
       </c>
       <c r="D173" t="n">
-        <v>44010</v>
+        <v>1075</v>
       </c>
       <c r="E173" t="b">
         <v>1</v>
@@ -6657,7 +6657,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.99975, -0.37823, -0.99973]), TrackedArray([0.99998, 0.72357, 1.     ]))</t>
+          <t>(TrackedArray([-0.99975, -0.37823, -0.99973]), TrackedArray([0.99998, 0.70757, 1.     ]))</t>
         </is>
       </c>
       <c r="H173" t="inlineStr">
@@ -6680,10 +6680,10 @@
         <v>4</v>
       </c>
       <c r="C174" t="n">
-        <v>2752</v>
+        <v>2000</v>
       </c>
       <c r="D174" t="n">
-        <v>1051</v>
+        <v>737</v>
       </c>
       <c r="E174" t="b">
         <v>1</v>
@@ -6702,10 +6702,10 @@
         </is>
       </c>
       <c r="I174" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J174" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175">
@@ -6716,10 +6716,10 @@
         <v>4</v>
       </c>
       <c r="C175" t="n">
-        <v>41835</v>
+        <v>1999</v>
       </c>
       <c r="D175" t="n">
-        <v>20981</v>
+        <v>1076</v>
       </c>
       <c r="E175" t="b">
         <v>1</v>
@@ -6729,7 +6729,7 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.89676, -0.60261, -0.84489]), TrackedArray([0.9057 , 1.     , 0.89885]))</t>
+          <t>(TrackedArray([-0.89713, -0.60261, -0.84489]), TrackedArray([0.90637, 0.98045, 0.89885]))</t>
         </is>
       </c>
       <c r="H175" t="inlineStr">
@@ -6752,10 +6752,10 @@
         <v>4</v>
       </c>
       <c r="C176" t="n">
-        <v>13978</v>
+        <v>2000</v>
       </c>
       <c r="D176" t="n">
-        <v>7223</v>
+        <v>1300</v>
       </c>
       <c r="E176" t="b">
         <v>1</v>
@@ -6765,7 +6765,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.47944, -0.33999, -0.46156]), TrackedArray([0.47798, 1.     , 0.46021]))</t>
+          <t>(TrackedArray([-0.47453, -0.33999, -0.45649]), TrackedArray([0.47306, 0.79664, 0.45514]))</t>
         </is>
       </c>
       <c r="H176" t="inlineStr">
@@ -6824,10 +6824,10 @@
         <v>4</v>
       </c>
       <c r="C178" t="n">
-        <v>2405</v>
+        <v>2000</v>
       </c>
       <c r="D178" t="n">
-        <v>1252</v>
+        <v>1091</v>
       </c>
       <c r="E178" t="b">
         <v>1</v>
@@ -6860,10 +6860,10 @@
         <v>4</v>
       </c>
       <c r="C179" t="n">
-        <v>2027</v>
+        <v>1998</v>
       </c>
       <c r="D179" t="n">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="E179" t="b">
         <v>1</v>
@@ -6896,10 +6896,10 @@
         <v>4</v>
       </c>
       <c r="C180" t="n">
-        <v>2076</v>
+        <v>2000</v>
       </c>
       <c r="D180" t="n">
-        <v>1217</v>
+        <v>1179</v>
       </c>
       <c r="E180" t="b">
         <v>1</v>
@@ -6932,10 +6932,10 @@
         <v>4</v>
       </c>
       <c r="C181" t="n">
-        <v>3922</v>
+        <v>2000</v>
       </c>
       <c r="D181" t="n">
-        <v>1952</v>
+        <v>1005</v>
       </c>
       <c r="E181" t="b">
         <v>1</v>
@@ -6968,10 +6968,10 @@
         <v>4</v>
       </c>
       <c r="C182" t="n">
-        <v>2820</v>
+        <v>2000</v>
       </c>
       <c r="D182" t="n">
-        <v>1990</v>
+        <v>1471</v>
       </c>
       <c r="E182" t="b">
         <v>1</v>
@@ -7148,10 +7148,10 @@
         <v>5</v>
       </c>
       <c r="C187" t="n">
-        <v>3450</v>
+        <v>2000</v>
       </c>
       <c r="D187" t="n">
-        <v>1725</v>
+        <v>1000</v>
       </c>
       <c r="E187" t="b">
         <v>1</v>
@@ -7184,10 +7184,10 @@
         <v>5</v>
       </c>
       <c r="C188" t="n">
-        <v>10370</v>
+        <v>2000</v>
       </c>
       <c r="D188" t="n">
-        <v>5183</v>
+        <v>1006</v>
       </c>
       <c r="E188" t="b">
         <v>1</v>
@@ -7197,7 +7197,7 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.83564, -0.61178, -0.95124]), TrackedArray([1.     , 0.6075 , 0.79626]))</t>
+          <t>(TrackedArray([-0.83524, -0.61094, -0.95124]), TrackedArray([0.99611, 0.60666, 0.79395]))</t>
         </is>
       </c>
       <c r="H188" t="inlineStr">
@@ -7220,10 +7220,10 @@
         <v>5</v>
       </c>
       <c r="C189" t="n">
-        <v>17597</v>
+        <v>2000</v>
       </c>
       <c r="D189" t="n">
-        <v>8692</v>
+        <v>1008</v>
       </c>
       <c r="E189" t="b">
         <v>1</v>
@@ -7233,7 +7233,7 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.5889 , -0.23957, -0.54998]), TrackedArray([1.     , 0.37073, 0.55002]))</t>
+          <t>(TrackedArray([-0.5889 , -0.23957, -0.54998]), TrackedArray([0.99915, 0.37066, 0.55002]))</t>
         </is>
       </c>
       <c r="H189" t="inlineStr">
@@ -7256,10 +7256,10 @@
         <v>5</v>
       </c>
       <c r="C190" t="n">
-        <v>6656</v>
+        <v>2000</v>
       </c>
       <c r="D190" t="n">
-        <v>3330</v>
+        <v>1003</v>
       </c>
       <c r="E190" t="b">
         <v>1</v>
@@ -7269,7 +7269,7 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.65683, -0.36894, -0.46426]), TrackedArray([1.     , 0.79963, 0.67327]))</t>
+          <t>(TrackedArray([-0.65683, -0.36887, -0.46426]), TrackedArray([1.     , 0.79963, 0.67327]))</t>
         </is>
       </c>
       <c r="H190" t="inlineStr">
@@ -7328,10 +7328,10 @@
         <v>5</v>
       </c>
       <c r="C192" t="n">
-        <v>11812</v>
+        <v>1999</v>
       </c>
       <c r="D192" t="n">
-        <v>5874</v>
+        <v>1002</v>
       </c>
       <c r="E192" t="b">
         <v>1</v>
@@ -7341,7 +7341,7 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.63394, -0.69443, -0.59245]), TrackedArray([1.     , 0.79206, 0.59318]))</t>
+          <t>(TrackedArray([-0.63325, -0.69443, -0.59245]), TrackedArray([0.99662, 0.79206, 0.59249]))</t>
         </is>
       </c>
       <c r="H192" t="inlineStr">
@@ -7364,10 +7364,10 @@
         <v>5</v>
       </c>
       <c r="C193" t="n">
-        <v>5252</v>
+        <v>1999</v>
       </c>
       <c r="D193" t="n">
-        <v>2653</v>
+        <v>1029</v>
       </c>
       <c r="E193" t="b">
         <v>1</v>
@@ -7377,7 +7377,7 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.21532,  0.29812, -0.18367]), TrackedArray([0.2166 , 1.     , 0.18353]))</t>
+          <t>(TrackedArray([-0.21532,  0.29812, -0.18367]), TrackedArray([0.2166 , 0.99984, 0.18353]))</t>
         </is>
       </c>
       <c r="H193" t="inlineStr">
@@ -7472,10 +7472,10 @@
         <v>6</v>
       </c>
       <c r="C196" t="n">
-        <v>59640</v>
+        <v>2000</v>
       </c>
       <c r="D196" t="n">
-        <v>30530</v>
+        <v>1046</v>
       </c>
       <c r="E196" t="b">
         <v>1</v>
@@ -7485,7 +7485,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.45499, -1.60366, -0.8583 ]), TrackedArray([ 0.45826, -0.1528 ,  1.     ]))</t>
+          <t>(TrackedArray([-0.45121, -1.60197, -0.85601]), TrackedArray([ 0.45319, -0.1545 ,  0.99779]))</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
@@ -7508,10 +7508,10 @@
         <v>6</v>
       </c>
       <c r="C197" t="n">
-        <v>16036</v>
+        <v>1999</v>
       </c>
       <c r="D197" t="n">
-        <v>9570</v>
+        <v>1179</v>
       </c>
       <c r="E197" t="b">
         <v>1</v>
@@ -7521,7 +7521,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.46591, -0.77449, -0.51799]), TrackedArray([1.     , 0.62957, 0.91896]))</t>
+          <t>(TrackedArray([-0.46134, -0.77448, -0.51785]), TrackedArray([1.     , 0.62896, 0.91894]))</t>
         </is>
       </c>
       <c r="H197" t="inlineStr">
@@ -7544,10 +7544,10 @@
         <v>6</v>
       </c>
       <c r="C198" t="n">
-        <v>10766</v>
+        <v>2000</v>
       </c>
       <c r="D198" t="n">
-        <v>5391</v>
+        <v>1008</v>
       </c>
       <c r="E198" t="b">
         <v>1</v>
@@ -7557,7 +7557,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.40246, -0.99439, -0.90838]), TrackedArray([0.44276, 1.     , 0.28458]))</t>
+          <t>(TrackedArray([-0.40226, -0.99439, -0.90838]), TrackedArray([0.44275, 1.     , 0.28458]))</t>
         </is>
       </c>
       <c r="H198" t="inlineStr">
@@ -7616,10 +7616,10 @@
         <v>6</v>
       </c>
       <c r="C200" t="n">
-        <v>2333</v>
+        <v>1999</v>
       </c>
       <c r="D200" t="n">
-        <v>1316</v>
+        <v>1149</v>
       </c>
       <c r="E200" t="b">
         <v>1</v>
@@ -7796,10 +7796,10 @@
         <v>6</v>
       </c>
       <c r="C205" t="n">
-        <v>2234</v>
+        <v>2000</v>
       </c>
       <c r="D205" t="n">
-        <v>1137</v>
+        <v>1020</v>
       </c>
       <c r="E205" t="b">
         <v>1</v>
@@ -7832,10 +7832,10 @@
         <v>6</v>
       </c>
       <c r="C206" t="n">
-        <v>8478</v>
+        <v>2000</v>
       </c>
       <c r="D206" t="n">
-        <v>4151</v>
+        <v>1011</v>
       </c>
       <c r="E206" t="b">
         <v>1</v>
@@ -7845,7 +7845,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.95956, -0.70677, -0.73536]), TrackedArray([1.     , 0.55719, 0.35128]))</t>
+          <t>(TrackedArray([-0.95956, -0.70677, -0.73536]), TrackedArray([1.     , 0.55518, 0.35125]))</t>
         </is>
       </c>
       <c r="H206" t="inlineStr">
@@ -8120,10 +8120,10 @@
         <v>7</v>
       </c>
       <c r="C214" t="n">
-        <v>15768</v>
+        <v>2000</v>
       </c>
       <c r="D214" t="n">
-        <v>7910</v>
+        <v>1028</v>
       </c>
       <c r="E214" t="b">
         <v>1</v>
@@ -8133,7 +8133,7 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.30294, -0.30266, -0.04749]), TrackedArray([0.30186, 1.     , 0.04795]))</t>
+          <t>(TrackedArray([-0.30081, -0.30266, -0.04715]), TrackedArray([0.29974, 1.     , 0.04784]))</t>
         </is>
       </c>
       <c r="H214" t="inlineStr">
@@ -8156,10 +8156,10 @@
         <v>7</v>
       </c>
       <c r="C215" t="n">
-        <v>9347</v>
+        <v>1994</v>
       </c>
       <c r="D215" t="n">
-        <v>3162</v>
+        <v>790</v>
       </c>
       <c r="E215" t="b">
         <v>1</v>
@@ -8169,7 +8169,7 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.02869,  0.63445,  0.12253]), TrackedArray([0.07113, 1.     , 0.14599]))</t>
+          <t>(TrackedArray([-0.02869,  0.63445,  0.1226 ]), TrackedArray([0.07113, 1.     , 0.14599]))</t>
         </is>
       </c>
       <c r="H215" t="inlineStr">
@@ -8178,10 +8178,10 @@
         </is>
       </c>
       <c r="I215" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J215" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216">
@@ -8192,10 +8192,10 @@
         <v>7</v>
       </c>
       <c r="C216" t="n">
-        <v>8628</v>
+        <v>2000</v>
       </c>
       <c r="D216" t="n">
-        <v>4325</v>
+        <v>1006</v>
       </c>
       <c r="E216" t="b">
         <v>1</v>
@@ -8205,7 +8205,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.19407, -0.47153, -0.03183]), TrackedArray([0.18515, 1.     , 0.031  ]))</t>
+          <t>(TrackedArray([-0.19398, -0.47153, -0.03178]), TrackedArray([0.18504, 1.     , 0.03089]))</t>
         </is>
       </c>
       <c r="H216" t="inlineStr">
@@ -8228,10 +8228,10 @@
         <v>7</v>
       </c>
       <c r="C217" t="n">
-        <v>3668</v>
+        <v>2000</v>
       </c>
       <c r="D217" t="n">
-        <v>1866</v>
+        <v>1032</v>
       </c>
       <c r="E217" t="b">
         <v>1</v>
@@ -8241,7 +8241,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.70608, -2.20481, -0.06603]), TrackedArray([0.70833, 1.     , 0.06617]))</t>
+          <t>(TrackedArray([-0.70566, -2.20481, -0.06603]), TrackedArray([0.70791, 1.     , 0.06617]))</t>
         </is>
       </c>
       <c r="H217" t="inlineStr">
@@ -8264,10 +8264,10 @@
         <v>7</v>
       </c>
       <c r="C218" t="n">
-        <v>13168</v>
+        <v>2000</v>
       </c>
       <c r="D218" t="n">
-        <v>6595</v>
+        <v>1014</v>
       </c>
       <c r="E218" t="b">
         <v>1</v>
@@ -8277,7 +8277,7 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.42888, -0.10768, -2.97758]), TrackedArray([0.42857, 0.10766, 1.     ]))</t>
+          <t>(TrackedArray([-0.42888, -0.10605, -2.97758]), TrackedArray([0.42857, 0.10603, 0.99756]))</t>
         </is>
       </c>
       <c r="H218" t="inlineStr">
@@ -8300,10 +8300,10 @@
         <v>7</v>
       </c>
       <c r="C219" t="n">
-        <v>21764</v>
+        <v>2000</v>
       </c>
       <c r="D219" t="n">
-        <v>10936</v>
+        <v>1048</v>
       </c>
       <c r="E219" t="b">
         <v>1</v>
@@ -8313,7 +8313,7 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.24657, -0.06202, -1.2822 ]), TrackedArray([0.22438, 0.06744, 1.     ]))</t>
+          <t>(TrackedArray([-0.24537, -0.05448, -1.2822 ]), TrackedArray([0.22409, 0.06509, 0.99625]))</t>
         </is>
       </c>
       <c r="H219" t="inlineStr">
@@ -8336,10 +8336,10 @@
         <v>7</v>
       </c>
       <c r="C220" t="n">
-        <v>17701</v>
+        <v>1999</v>
       </c>
       <c r="D220" t="n">
-        <v>9445</v>
+        <v>1144</v>
       </c>
       <c r="E220" t="b">
         <v>1</v>
@@ -8349,7 +8349,7 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.18064, -0.03433, -0.69698]), TrackedArray([0.18327, 0.02033, 1.     ]))</t>
+          <t>(TrackedArray([-0.18064, -0.03433, -0.69697]), TrackedArray([0.18327, 0.02033, 0.993  ]))</t>
         </is>
       </c>
       <c r="H220" t="inlineStr">
@@ -8372,10 +8372,10 @@
         <v>7</v>
       </c>
       <c r="C221" t="n">
-        <v>9314</v>
+        <v>1999</v>
       </c>
       <c r="D221" t="n">
-        <v>4876</v>
+        <v>1098</v>
       </c>
       <c r="E221" t="b">
         <v>1</v>
@@ -8385,7 +8385,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>(TrackedArray([-2.21052, -0.07375, -0.31418]), TrackedArray([1.     , 0.0327 , 0.30768]))</t>
+          <t>(TrackedArray([-2.21052, -0.07375, -0.3138 ]), TrackedArray([0.99991, 0.0327 , 0.3073 ]))</t>
         </is>
       </c>
       <c r="H221" t="inlineStr">
@@ -8444,10 +8444,10 @@
         <v>8</v>
       </c>
       <c r="C223" t="n">
-        <v>16268</v>
+        <v>2000</v>
       </c>
       <c r="D223" t="n">
-        <v>8188</v>
+        <v>1054</v>
       </c>
       <c r="E223" t="b">
         <v>1</v>
@@ -8457,7 +8457,7 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.51756, -1.15069, -0.4365 ]), TrackedArray([0.48842, 1.     , 0.74077]))</t>
+          <t>(TrackedArray([-0.51344, -1.14932, -0.4365 ]), TrackedArray([0.48306, 1.     , 0.73917]))</t>
         </is>
       </c>
       <c r="H223" t="inlineStr">
@@ -8516,10 +8516,10 @@
         <v>8</v>
       </c>
       <c r="C225" t="n">
-        <v>2481</v>
+        <v>1999</v>
       </c>
       <c r="D225" t="n">
-        <v>1318</v>
+        <v>1057</v>
       </c>
       <c r="E225" t="b">
         <v>1</v>
@@ -8529,7 +8529,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>(TrackedArray([ -0.92905, -24.80653,  -2.53683]), TrackedArray([  1.     , -21.4446 ,  -0.47788]))</t>
+          <t>(TrackedArray([ -0.92905, -24.80653,  -2.53319]), TrackedArray([  1.     , -21.4446 ,  -0.47788]))</t>
         </is>
       </c>
       <c r="H225" t="inlineStr">
@@ -9200,10 +9200,10 @@
         <v>9</v>
       </c>
       <c r="C244" t="n">
-        <v>3048</v>
+        <v>2000</v>
       </c>
       <c r="D244" t="n">
-        <v>1586</v>
+        <v>1010</v>
       </c>
       <c r="E244" t="b">
         <v>1</v>
@@ -9213,7 +9213,7 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>(TrackedArray([-0.71428, -0.78685, -1.     ]), TrackedArray([0.71429, 0.09479, 1.     ]))</t>
+          <t>(TrackedArray([-0.71428, -0.78426, -1.     ]), TrackedArray([0.71429, 0.09479, 1.     ]))</t>
         </is>
       </c>
       <c r="H244" t="inlineStr">

</xml_diff>

<commit_message>
eat pasta run fasta
</commit_message>
<xml_diff>
--- a/features/refined.xlsx
+++ b/features/refined.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L242"/>
+  <dimension ref="A1:L245"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7935,7 +7935,7 @@
         <v>2000</v>
       </c>
       <c r="D179" t="n">
-        <v>1472</v>
+        <v>1179</v>
       </c>
       <c r="E179" t="b">
         <v>1</v>
@@ -7945,19 +7945,19 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.12811, 0.51158]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.44198, 0.94572]))</t>
         </is>
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t>testModels/refined_db/4/m412/m412.off</t>
+          <t>testModels/refined_db/4/m410/m410.off</t>
         </is>
       </c>
       <c r="I179" t="n">
-        <v>0.02426980825759749</v>
+        <v>0.4426165134704702</v>
       </c>
       <c r="J179" t="n">
-        <v>0.04766319038249999</v>
+        <v>0.36472700513595</v>
       </c>
       <c r="K179" t="b">
         <v>0</v>
@@ -7971,13 +7971,13 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C180" t="n">
-        <v>1996</v>
+        <v>2000</v>
       </c>
       <c r="D180" t="n">
-        <v>1000</v>
+        <v>1009</v>
       </c>
       <c r="E180" t="b">
         <v>1</v>
@@ -7987,19 +7987,19 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.95964, 0.89686, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.70357, 0.45049]))</t>
         </is>
       </c>
       <c r="H180" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m500/m500.off</t>
+          <t>testModels/refined_db/4/m411/m411.off</t>
         </is>
       </c>
       <c r="I180" t="n">
-        <v>0.0006964191987781477</v>
+        <v>0.356823088341781</v>
       </c>
       <c r="J180" t="n">
-        <v>0.774133244696</v>
+        <v>0.2742882714080499</v>
       </c>
       <c r="K180" t="b">
         <v>0</v>
@@ -8013,13 +8013,13 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C181" t="n">
         <v>2000</v>
       </c>
       <c r="D181" t="n">
-        <v>1072</v>
+        <v>1472</v>
       </c>
       <c r="E181" t="b">
         <v>1</v>
@@ -8029,25 +8029,25 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.67754, 0.975  , 0.67754]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.12811, 0.51158]))</t>
         </is>
       </c>
       <c r="H181" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m501/m501.off</t>
+          <t>testModels/refined_db/4/m412/m412.off</t>
         </is>
       </c>
       <c r="I181" t="n">
-        <v>0.0001625845650226333</v>
+        <v>0.02426980825759749</v>
       </c>
       <c r="J181" t="n">
-        <v>0.4045155493718</v>
+        <v>0.04766319038249999</v>
       </c>
       <c r="K181" t="b">
         <v>0</v>
       </c>
       <c r="L181" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182">
@@ -8071,19 +8071,19 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.67501, 0.975  , 0.67501]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.95964, 0.89686, 0.975  ]))</t>
         </is>
       </c>
       <c r="H182" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m502/m502.off</t>
+          <t>testModels/refined_db/5/m500/m500.off</t>
         </is>
       </c>
       <c r="I182" t="n">
-        <v>0.002764792734748884</v>
+        <v>0.0006964191987781477</v>
       </c>
       <c r="J182" t="n">
-        <v>0.4013836450465499</v>
+        <v>0.774133244696</v>
       </c>
       <c r="K182" t="b">
         <v>0</v>
@@ -8100,10 +8100,10 @@
         <v>5</v>
       </c>
       <c r="C183" t="n">
-        <v>1952</v>
+        <v>2000</v>
       </c>
       <c r="D183" t="n">
-        <v>1000</v>
+        <v>1072</v>
       </c>
       <c r="E183" t="b">
         <v>1</v>
@@ -8113,19 +8113,19 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.8853, 0.975 , 0.5708]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.67754, 0.975  , 0.67754]))</t>
         </is>
       </c>
       <c r="H183" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m503/m503.off</t>
+          <t>testModels/refined_db/5/m501/m501.off</t>
         </is>
       </c>
       <c r="I183" t="n">
-        <v>0.002016172263500733</v>
+        <v>0.0001625845650226333</v>
       </c>
       <c r="J183" t="n">
-        <v>0.44607162209075</v>
+        <v>0.4045155493718</v>
       </c>
       <c r="K183" t="b">
         <v>0</v>
@@ -8142,7 +8142,7 @@
         <v>5</v>
       </c>
       <c r="C184" t="n">
-        <v>2000</v>
+        <v>1996</v>
       </c>
       <c r="D184" t="n">
         <v>1000</v>
@@ -8155,19 +8155,19 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.73697, 0.77026]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.67501, 0.975  , 0.67501]))</t>
         </is>
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m504/m504.off</t>
+          <t>testModels/refined_db/5/m502/m502.off</t>
         </is>
       </c>
       <c r="I184" t="n">
-        <v>2.155574185068136e-05</v>
+        <v>0.002764792734748884</v>
       </c>
       <c r="J184" t="n">
-        <v>0.50407117646765</v>
+        <v>0.4013836450465499</v>
       </c>
       <c r="K184" t="b">
         <v>0</v>
@@ -8184,10 +8184,10 @@
         <v>5</v>
       </c>
       <c r="C185" t="n">
-        <v>2000</v>
+        <v>1952</v>
       </c>
       <c r="D185" t="n">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="E185" t="b">
         <v>1</v>
@@ -8197,19 +8197,19 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.02521, 0.02544, 0.025  ]), TrackedArray([0.97299, 0.65558, 0.92819]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.8853, 0.975 , 0.5708]))</t>
         </is>
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m505/m505.off</t>
+          <t>testModels/refined_db/5/m503/m503.off</t>
         </is>
       </c>
       <c r="I185" t="n">
-        <v>0.00526397823374702</v>
+        <v>0.002016172263500733</v>
       </c>
       <c r="J185" t="n">
-        <v>0.5394184393397173</v>
+        <v>0.44607162209075</v>
       </c>
       <c r="K185" t="b">
         <v>0</v>
@@ -8229,7 +8229,7 @@
         <v>2000</v>
       </c>
       <c r="D186" t="n">
-        <v>1008</v>
+        <v>1000</v>
       </c>
       <c r="E186" t="b">
         <v>1</v>
@@ -8239,19 +8239,19 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.97449, 0.38986, 0.68268]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.73697, 0.77026]))</t>
         </is>
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m506/m506.off</t>
+          <t>testModels/refined_db/5/m504/m504.off</t>
         </is>
       </c>
       <c r="I186" t="n">
-        <v>0.0003049739221834936</v>
+        <v>2.155574185068136e-05</v>
       </c>
       <c r="J186" t="n">
-        <v>0.2278390717677797</v>
+        <v>0.50407117646765</v>
       </c>
       <c r="K186" t="b">
         <v>0</v>
@@ -8281,19 +8281,19 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025  , 0.02504, 0.025  ]), TrackedArray([0.975  , 0.69504, 0.67724]))</t>
+          <t>(TrackedArray([0.02521, 0.02544, 0.025  ]), TrackedArray([0.97299, 0.65558, 0.92819]))</t>
         </is>
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m507/m507.off</t>
+          <t>testModels/refined_db/5/m505/m505.off</t>
         </is>
       </c>
       <c r="I187" t="n">
-        <v>0.0004915109394796224</v>
+        <v>0.00526397823374702</v>
       </c>
       <c r="J187" t="n">
-        <v>0.415150557238935</v>
+        <v>0.5394184393397173</v>
       </c>
       <c r="K187" t="b">
         <v>0</v>
@@ -8310,10 +8310,10 @@
         <v>5</v>
       </c>
       <c r="C188" t="n">
-        <v>1988</v>
+        <v>2000</v>
       </c>
       <c r="D188" t="n">
-        <v>998</v>
+        <v>1008</v>
       </c>
       <c r="E188" t="b">
         <v>1</v>
@@ -8323,19 +8323,19 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.80951, 0.62492]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.97449, 0.38986, 0.68268]))</t>
         </is>
       </c>
       <c r="H188" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m508/m508.off</t>
+          <t>testModels/refined_db/5/m506/m506.off</t>
         </is>
       </c>
       <c r="I188" t="n">
-        <v>2.593299697940728e-05</v>
+        <v>0.0003049739221834936</v>
       </c>
       <c r="J188" t="n">
-        <v>0.4471125239474999</v>
+        <v>0.2278390717677797</v>
       </c>
       <c r="K188" t="b">
         <v>0</v>
@@ -8352,10 +8352,10 @@
         <v>5</v>
       </c>
       <c r="C189" t="n">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="D189" t="n">
-        <v>1002</v>
+        <v>1006</v>
       </c>
       <c r="E189" t="b">
         <v>1</v>
@@ -8365,19 +8365,19 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.0254, 0.025 , 0.025 ]), TrackedArray([0.97303, 0.88927, 0.71394]))</t>
+          <t>(TrackedArray([0.025  , 0.02504, 0.025  ]), TrackedArray([0.975  , 0.69504, 0.67724]))</t>
         </is>
       </c>
       <c r="H189" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m509/m509.off</t>
+          <t>testModels/refined_db/5/m507/m507.off</t>
         </is>
       </c>
       <c r="I189" t="n">
-        <v>0.001541805271098911</v>
+        <v>0.0004915109394796224</v>
       </c>
       <c r="J189" t="n">
-        <v>0.5642497394150771</v>
+        <v>0.415150557238935</v>
       </c>
       <c r="K189" t="b">
         <v>0</v>
@@ -8394,10 +8394,10 @@
         <v>5</v>
       </c>
       <c r="C190" t="n">
-        <v>1999</v>
+        <v>1988</v>
       </c>
       <c r="D190" t="n">
-        <v>1035</v>
+        <v>998</v>
       </c>
       <c r="E190" t="b">
         <v>1</v>
@@ -8407,19 +8407,19 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.60961, 0.97479, 0.52201]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.80951, 0.62492]))</t>
         </is>
       </c>
       <c r="H190" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m510/m510.off</t>
+          <t>testModels/refined_db/5/m508/m508.off</t>
         </is>
       </c>
       <c r="I190" t="n">
-        <v>0.0004058991979104314</v>
+        <v>2.593299697940728e-05</v>
       </c>
       <c r="J190" t="n">
-        <v>0.2759672917384885</v>
+        <v>0.4471125239474999</v>
       </c>
       <c r="K190" t="b">
         <v>0</v>
@@ -8436,10 +8436,10 @@
         <v>5</v>
       </c>
       <c r="C191" t="n">
-        <v>2202</v>
+        <v>1999</v>
       </c>
       <c r="D191" t="n">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E191" t="b">
         <v>1</v>
@@ -8449,19 +8449,19 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.9522 , 0.975  , 0.92067]))</t>
+          <t>(TrackedArray([0.0254, 0.025 , 0.025 ]), TrackedArray([0.97303, 0.88927, 0.71394]))</t>
         </is>
       </c>
       <c r="H191" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m511/m511.off</t>
+          <t>testModels/refined_db/5/m509/m509.off</t>
         </is>
       </c>
       <c r="I191" t="n">
-        <v>0.02789926138668109</v>
+        <v>0.001541805271098911</v>
       </c>
       <c r="J191" t="n">
-        <v>0.7889463070987</v>
+        <v>0.5642497394150771</v>
       </c>
       <c r="K191" t="b">
         <v>0</v>
@@ -8478,10 +8478,10 @@
         <v>5</v>
       </c>
       <c r="C192" t="n">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="D192" t="n">
-        <v>1000</v>
+        <v>1035</v>
       </c>
       <c r="E192" t="b">
         <v>1</v>
@@ -8491,19 +8491,19 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.79759, 0.975  , 0.79759]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.60961, 0.97479, 0.52201]))</t>
         </is>
       </c>
       <c r="H192" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m512/m512.off</t>
+          <t>testModels/refined_db/5/m510/m510.off</t>
         </is>
       </c>
       <c r="I192" t="n">
-        <v>0.003047668860747743</v>
+        <v>0.0004058991979104314</v>
       </c>
       <c r="J192" t="n">
-        <v>0.56704613894055</v>
+        <v>0.2759672917384885</v>
       </c>
       <c r="K192" t="b">
         <v>0</v>
@@ -8517,13 +8517,13 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C193" t="n">
-        <v>2000</v>
+        <v>2202</v>
       </c>
       <c r="D193" t="n">
-        <v>1042</v>
+        <v>1000</v>
       </c>
       <c r="E193" t="b">
         <v>1</v>
@@ -8533,19 +8533,19 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.02693, 0.02586, 0.02617]), TrackedArray([0.48928, 0.76584, 0.97387]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.9522 , 0.975  , 0.92067]))</t>
         </is>
       </c>
       <c r="H193" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m600/m600.off</t>
+          <t>testModels/refined_db/5/m511/m511.off</t>
         </is>
       </c>
       <c r="I193" t="n">
-        <v>0.002188264251238722</v>
+        <v>0.02789926138668109</v>
       </c>
       <c r="J193" t="n">
-        <v>0.3242315189462048</v>
+        <v>0.7889463070987</v>
       </c>
       <c r="K193" t="b">
         <v>0</v>
@@ -8559,13 +8559,13 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C194" t="n">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="D194" t="n">
-        <v>1175</v>
+        <v>1000</v>
       </c>
       <c r="E194" t="b">
         <v>1</v>
@@ -8575,25 +8575,25 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.02796, 0.02501, 0.02509]), TrackedArray([0.975  , 0.93453, 0.95622]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.79759, 0.975  , 0.79759]))</t>
         </is>
       </c>
       <c r="H194" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m601/m601.off</t>
+          <t>testModels/refined_db/5/m512/m512.off</t>
         </is>
       </c>
       <c r="I194" t="n">
-        <v>0.001129485291517668</v>
+        <v>0.003047668860747743</v>
       </c>
       <c r="J194" t="n">
-        <v>0.8020325620060286</v>
+        <v>0.56704613894055</v>
       </c>
       <c r="K194" t="b">
         <v>0</v>
       </c>
       <c r="L194" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195">
@@ -8607,7 +8607,7 @@
         <v>2000</v>
       </c>
       <c r="D195" t="n">
-        <v>1008</v>
+        <v>1042</v>
       </c>
       <c r="E195" t="b">
         <v>1</v>
@@ -8617,19 +8617,19 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.02509, 0.025  , 0.025  ]), TrackedArray([0.4276 , 0.975  , 0.59325]))</t>
+          <t>(TrackedArray([0.02693, 0.02586, 0.02617]), TrackedArray([0.48928, 0.76584, 0.97387]))</t>
         </is>
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m602/m602.off</t>
+          <t>testModels/refined_db/6/m600/m600.off</t>
         </is>
       </c>
       <c r="I195" t="n">
-        <v>0.0007723776362440639</v>
+        <v>0.002188264251238722</v>
       </c>
       <c r="J195" t="n">
-        <v>0.217290235051875</v>
+        <v>0.3242315189462048</v>
       </c>
       <c r="K195" t="b">
         <v>0</v>
@@ -8646,10 +8646,10 @@
         <v>6</v>
       </c>
       <c r="C196" t="n">
-        <v>1996</v>
+        <v>1999</v>
       </c>
       <c r="D196" t="n">
-        <v>1000</v>
+        <v>1175</v>
       </c>
       <c r="E196" t="b">
         <v>1</v>
@@ -8659,25 +8659,25 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.58332, 0.84655, 0.975  ]))</t>
+          <t>(TrackedArray([0.02796, 0.02501, 0.02509]), TrackedArray([0.975  , 0.93453, 0.95622]))</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m603/m603.off</t>
+          <t>testModels/refined_db/6/m601/m601.off</t>
         </is>
       </c>
       <c r="I196" t="n">
-        <v>0.000745184319603115</v>
+        <v>0.001129485291517668</v>
       </c>
       <c r="J196" t="n">
-        <v>0.4357544367391</v>
+        <v>0.8020325620060286</v>
       </c>
       <c r="K196" t="b">
         <v>0</v>
       </c>
       <c r="L196" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197">
@@ -8688,10 +8688,10 @@
         <v>6</v>
       </c>
       <c r="C197" t="n">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="D197" t="n">
-        <v>1149</v>
+        <v>1008</v>
       </c>
       <c r="E197" t="b">
         <v>1</v>
@@ -8701,25 +8701,25 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.69906, 0.975  , 0.15606]))</t>
+          <t>(TrackedArray([0.02509, 0.025  , 0.025  ]), TrackedArray([0.4276 , 0.975  , 0.59325]))</t>
         </is>
       </c>
       <c r="H197" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m604/m604.off</t>
+          <t>testModels/refined_db/6/m602/m602.off</t>
         </is>
       </c>
       <c r="I197" t="n">
-        <v>0.02392622713249805</v>
+        <v>0.0007723776362440639</v>
       </c>
       <c r="J197" t="n">
-        <v>0.083922626992</v>
+        <v>0.217290235051875</v>
       </c>
       <c r="K197" t="b">
         <v>0</v>
       </c>
       <c r="L197" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198">
@@ -8730,10 +8730,10 @@
         <v>6</v>
       </c>
       <c r="C198" t="n">
-        <v>2238</v>
+        <v>1996</v>
       </c>
       <c r="D198" t="n">
-        <v>834</v>
+        <v>1000</v>
       </c>
       <c r="E198" t="b">
         <v>1</v>
@@ -8743,22 +8743,22 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.50208, 0.975  , 0.83687]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.58332, 0.84655, 0.975  ]))</t>
         </is>
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m605/m605.off</t>
+          <t>testModels/refined_db/6/m603/m603.off</t>
         </is>
       </c>
       <c r="I198" t="n">
-        <v>0.002287657914562828</v>
+        <v>0.000745184319603115</v>
       </c>
       <c r="J198" t="n">
-        <v>0.36795691912105</v>
+        <v>0.4357544367391</v>
       </c>
       <c r="K198" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L198" t="b">
         <v>0</v>
@@ -8772,10 +8772,10 @@
         <v>6</v>
       </c>
       <c r="C199" t="n">
-        <v>1971</v>
+        <v>1999</v>
       </c>
       <c r="D199" t="n">
-        <v>1000</v>
+        <v>1149</v>
       </c>
       <c r="E199" t="b">
         <v>1</v>
@@ -8785,25 +8785,25 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.83864, 0.975  , 0.45899]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.69906, 0.975  , 0.15606]))</t>
         </is>
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m606/m606.off</t>
+          <t>testModels/refined_db/6/m604/m604.off</t>
         </is>
       </c>
       <c r="I199" t="n">
-        <v>0.01730747197990135</v>
+        <v>0.02392622713249805</v>
       </c>
       <c r="J199" t="n">
-        <v>0.3354520743954</v>
+        <v>0.083922626992</v>
       </c>
       <c r="K199" t="b">
         <v>0</v>
       </c>
       <c r="L199" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200">
@@ -8814,10 +8814,10 @@
         <v>6</v>
       </c>
       <c r="C200" t="n">
-        <v>1709</v>
+        <v>2238</v>
       </c>
       <c r="D200" t="n">
-        <v>901</v>
+        <v>834</v>
       </c>
       <c r="E200" t="b">
         <v>1</v>
@@ -8827,22 +8827,22 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.34539, 0.975  , 0.84361]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.50208, 0.975  , 0.83687]))</t>
         </is>
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m607/m607.off</t>
+          <t>testModels/refined_db/6/m605/m605.off</t>
         </is>
       </c>
       <c r="I200" t="n">
-        <v>1.595780916046108e-05</v>
+        <v>0.002287657914562828</v>
       </c>
       <c r="J200" t="n">
-        <v>0.2491597883831999</v>
+        <v>0.36795691912105</v>
       </c>
       <c r="K200" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L200" t="b">
         <v>0</v>
@@ -8856,7 +8856,7 @@
         <v>6</v>
       </c>
       <c r="C201" t="n">
-        <v>1916</v>
+        <v>1971</v>
       </c>
       <c r="D201" t="n">
         <v>1000</v>
@@ -8869,19 +8869,19 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.75998, 0.90819, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.83864, 0.975  , 0.45899]))</t>
         </is>
       </c>
       <c r="H201" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m608/m608.off</t>
+          <t>testModels/refined_db/6/m606/m606.off</t>
         </is>
       </c>
       <c r="I201" t="n">
-        <v>8.632235975886356e-05</v>
+        <v>0.01730747197990135</v>
       </c>
       <c r="J201" t="n">
-        <v>0.6166739930119999</v>
+        <v>0.3354520743954</v>
       </c>
       <c r="K201" t="b">
         <v>0</v>
@@ -8898,10 +8898,10 @@
         <v>6</v>
       </c>
       <c r="C202" t="n">
-        <v>2000</v>
+        <v>1709</v>
       </c>
       <c r="D202" t="n">
-        <v>1020</v>
+        <v>901</v>
       </c>
       <c r="E202" t="b">
         <v>1</v>
@@ -8911,19 +8911,19 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.21256, 0.72068, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.34539, 0.975  , 0.84361]))</t>
         </is>
       </c>
       <c r="H202" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m609/m609.off</t>
+          <t>testModels/refined_db/6/m607/m607.off</t>
         </is>
       </c>
       <c r="I202" t="n">
-        <v>0.0003560311298754342</v>
+        <v>1.595780916046108e-05</v>
       </c>
       <c r="J202" t="n">
-        <v>0.1239595846008</v>
+        <v>0.2491597883831999</v>
       </c>
       <c r="K202" t="b">
         <v>0</v>
@@ -8940,10 +8940,10 @@
         <v>6</v>
       </c>
       <c r="C203" t="n">
-        <v>2000</v>
+        <v>1916</v>
       </c>
       <c r="D203" t="n">
-        <v>1016</v>
+        <v>1000</v>
       </c>
       <c r="E203" t="b">
         <v>1</v>
@@ -8953,19 +8953,19 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.6368 , 0.55179]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.75998, 0.90819, 0.975  ]))</t>
         </is>
       </c>
       <c r="H203" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m610/m610.off</t>
+          <t>testModels/refined_db/6/m608/m608.off</t>
         </is>
       </c>
       <c r="I203" t="n">
-        <v>1.331384143935641e-05</v>
+        <v>8.632235975886356e-05</v>
       </c>
       <c r="J203" t="n">
-        <v>0.3061758177928125</v>
+        <v>0.6166739930119999</v>
       </c>
       <c r="K203" t="b">
         <v>0</v>
@@ -8982,10 +8982,10 @@
         <v>6</v>
       </c>
       <c r="C204" t="n">
-        <v>2026</v>
+        <v>2000</v>
       </c>
       <c r="D204" t="n">
-        <v>778</v>
+        <v>1020</v>
       </c>
       <c r="E204" t="b">
         <v>1</v>
@@ -8995,22 +8995,22 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.84401, 0.975  , 0.45893]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.21256, 0.72068, 0.975  ]))</t>
         </is>
       </c>
       <c r="H204" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m611/m611.off</t>
+          <t>testModels/refined_db/6/m609/m609.off</t>
         </is>
       </c>
       <c r="I204" t="n">
-        <v>0.006340770550030407</v>
+        <v>0.0003560311298754342</v>
       </c>
       <c r="J204" t="n">
-        <v>0.337626976131</v>
+        <v>0.1239595846008</v>
       </c>
       <c r="K204" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L204" t="b">
         <v>0</v>
@@ -9024,10 +9024,10 @@
         <v>6</v>
       </c>
       <c r="C205" t="n">
-        <v>2232</v>
+        <v>2000</v>
       </c>
       <c r="D205" t="n">
-        <v>948</v>
+        <v>1016</v>
       </c>
       <c r="E205" t="b">
         <v>1</v>
@@ -9037,19 +9037,19 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.75993, 0.90811, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.6368 , 0.55179]))</t>
         </is>
       </c>
       <c r="H205" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m612/m612.off</t>
+          <t>testModels/refined_db/6/m610/m610.off</t>
         </is>
       </c>
       <c r="I205" t="n">
-        <v>0.0001209419976838267</v>
+        <v>1.331384143935641e-05</v>
       </c>
       <c r="J205" t="n">
-        <v>0.6165689174602</v>
+        <v>0.3061758177928125</v>
       </c>
       <c r="K205" t="b">
         <v>0</v>
@@ -9063,13 +9063,13 @@
         <v>204</v>
       </c>
       <c r="B206" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C206" t="n">
-        <v>1904</v>
+        <v>2026</v>
       </c>
       <c r="D206" t="n">
-        <v>1000</v>
+        <v>778</v>
       </c>
       <c r="E206" t="b">
         <v>1</v>
@@ -9079,22 +9079,22 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.41837, 0.975  , 0.09773]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.84401, 0.975  , 0.45893]))</t>
         </is>
       </c>
       <c r="H206" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m700/m700.off</t>
+          <t>testModels/refined_db/6/m611/m611.off</t>
         </is>
       </c>
       <c r="I206" t="n">
-        <v>0.001634965579034274</v>
+        <v>0.006340770550030407</v>
       </c>
       <c r="J206" t="n">
-        <v>0.027180761887565</v>
+        <v>0.337626976131</v>
       </c>
       <c r="K206" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L206" t="b">
         <v>0</v>
@@ -9105,13 +9105,13 @@
         <v>205</v>
       </c>
       <c r="B207" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C207" t="n">
-        <v>1900</v>
+        <v>2232</v>
       </c>
       <c r="D207" t="n">
-        <v>960</v>
+        <v>948</v>
       </c>
       <c r="E207" t="b">
         <v>1</v>
@@ -9121,19 +9121,19 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.04405, 0.30701, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.75993, 0.90811, 0.975  ]))</t>
         </is>
       </c>
       <c r="H207" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m701/m701.off</t>
+          <t>testModels/refined_db/6/m612/m612.off</t>
         </is>
       </c>
       <c r="I207" t="n">
-        <v>0.0005984744284004732</v>
+        <v>0.0001209419976838267</v>
       </c>
       <c r="J207" t="n">
-        <v>0.005102765082699999</v>
+        <v>0.6165689174602</v>
       </c>
       <c r="K207" t="b">
         <v>0</v>
@@ -9150,10 +9150,10 @@
         <v>7</v>
       </c>
       <c r="C208" t="n">
-        <v>2000</v>
+        <v>1904</v>
       </c>
       <c r="D208" t="n">
-        <v>1005</v>
+        <v>1000</v>
       </c>
       <c r="E208" t="b">
         <v>1</v>
@@ -9163,19 +9163,19 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.12358, 0.12358, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.41837, 0.975  , 0.09773]))</t>
         </is>
       </c>
       <c r="H208" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m702/m702.off</t>
+          <t>testModels/refined_db/7/m700/m700.off</t>
         </is>
       </c>
       <c r="I208" t="n">
-        <v>0.0002847790346095218</v>
+        <v>0.001634965579034274</v>
       </c>
       <c r="J208" t="n">
-        <v>0.0092317409798</v>
+        <v>0.027180761887565</v>
       </c>
       <c r="K208" t="b">
         <v>0</v>
@@ -9192,10 +9192,10 @@
         <v>7</v>
       </c>
       <c r="C209" t="n">
-        <v>1924</v>
+        <v>1900</v>
       </c>
       <c r="D209" t="n">
-        <v>1000</v>
+        <v>960</v>
       </c>
       <c r="E209" t="b">
         <v>1</v>
@@ -9205,19 +9205,19 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.05076, 0.12084, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.04405, 0.30701, 0.975  ]))</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m703/m703.off</t>
+          <t>testModels/refined_db/7/m701/m701.off</t>
         </is>
       </c>
       <c r="I209" t="n">
-        <v>0.0001905921691495498</v>
+        <v>0.0005984744284004732</v>
       </c>
       <c r="J209" t="n">
-        <v>0.002345430056895</v>
+        <v>0.005102765082699999</v>
       </c>
       <c r="K209" t="b">
         <v>0</v>
@@ -9234,10 +9234,10 @@
         <v>7</v>
       </c>
       <c r="C210" t="n">
-        <v>1996</v>
+        <v>2000</v>
       </c>
       <c r="D210" t="n">
-        <v>1000</v>
+        <v>1005</v>
       </c>
       <c r="E210" t="b">
         <v>1</v>
@@ -9247,19 +9247,19 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.05493, 0.08613, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.12358, 0.12358, 0.975  ]))</t>
         </is>
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m704/m704.off</t>
+          <t>testModels/refined_db/7/m702/m702.off</t>
         </is>
       </c>
       <c r="I210" t="n">
-        <v>9.025291300841998e-05</v>
+        <v>0.0002847790346095218</v>
       </c>
       <c r="J210" t="n">
-        <v>0.001738359126875</v>
+        <v>0.0092317409798</v>
       </c>
       <c r="K210" t="b">
         <v>0</v>
@@ -9276,10 +9276,10 @@
         <v>7</v>
       </c>
       <c r="C211" t="n">
-        <v>2000</v>
+        <v>1924</v>
       </c>
       <c r="D211" t="n">
-        <v>1028</v>
+        <v>1000</v>
       </c>
       <c r="E211" t="b">
         <v>1</v>
@@ -9289,19 +9289,19 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.02655, 0.025  , 0.02525]), TrackedArray([0.46452, 0.975  , 0.09452]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.05076, 0.12084, 0.975  ]))</t>
         </is>
       </c>
       <c r="H211" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m705/m705.off</t>
+          <t>testModels/refined_db/7/m703/m703.off</t>
         </is>
       </c>
       <c r="I211" t="n">
-        <v>0.0005383789458012969</v>
+        <v>0.0001905921691495498</v>
       </c>
       <c r="J211" t="n">
-        <v>0.02882194424788575</v>
+        <v>0.002345430056895</v>
       </c>
       <c r="K211" t="b">
         <v>0</v>
@@ -9318,10 +9318,10 @@
         <v>7</v>
       </c>
       <c r="C212" t="n">
-        <v>1999</v>
+        <v>1996</v>
       </c>
       <c r="D212" t="n">
-        <v>802</v>
+        <v>1000</v>
       </c>
       <c r="E212" t="b">
         <v>1</v>
@@ -9331,22 +9331,22 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025 , 0.025 , 0.0252]), TrackedArray([0.28441, 0.975  , 0.08598]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.05493, 0.08613, 0.975  ]))</t>
         </is>
       </c>
       <c r="H212" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m706/m706.off</t>
+          <t>testModels/refined_db/7/m704/m704.off</t>
         </is>
       </c>
       <c r="I212" t="n">
-        <v>0.000843582869486666</v>
+        <v>9.025291300841998e-05</v>
       </c>
       <c r="J212" t="n">
-        <v>0.01497704798992</v>
+        <v>0.001738359126875</v>
       </c>
       <c r="K212" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L212" t="b">
         <v>0</v>
@@ -9360,10 +9360,10 @@
         <v>7</v>
       </c>
       <c r="C213" t="n">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="D213" t="n">
-        <v>1005</v>
+        <v>1028</v>
       </c>
       <c r="E213" t="b">
         <v>1</v>
@@ -9373,19 +9373,19 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.02506, 0.025  , 0.02503]), TrackedArray([0.26975, 0.975  , 0.06549]))</t>
+          <t>(TrackedArray([0.02655, 0.025  , 0.02525]), TrackedArray([0.46452, 0.975  , 0.09452]))</t>
         </is>
       </c>
       <c r="H213" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m707/m707.off</t>
+          <t>testModels/refined_db/7/m705/m705.off</t>
         </is>
       </c>
       <c r="I213" t="n">
-        <v>0.06494472469930278</v>
+        <v>0.0005383789458012969</v>
       </c>
       <c r="J213" t="n">
-        <v>0.009405908309349748</v>
+        <v>0.02882194424788575</v>
       </c>
       <c r="K213" t="b">
         <v>0</v>
@@ -9402,10 +9402,10 @@
         <v>7</v>
       </c>
       <c r="C214" t="n">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="D214" t="n">
-        <v>1032</v>
+        <v>802</v>
       </c>
       <c r="E214" t="b">
         <v>1</v>
@@ -9415,22 +9415,22 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.02512, 0.025  , 0.025  ]), TrackedArray([0.44415, 0.975  , 0.06419]))</t>
+          <t>(TrackedArray([0.025 , 0.025 , 0.0252]), TrackedArray([0.28441, 0.975  , 0.08598]))</t>
         </is>
       </c>
       <c r="H214" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m708/m708.off</t>
+          <t>testModels/refined_db/7/m706/m706.off</t>
         </is>
       </c>
       <c r="I214" t="n">
-        <v>0.004282833850689033</v>
+        <v>0.000843582869486666</v>
       </c>
       <c r="J214" t="n">
-        <v>0.01559969183422879</v>
+        <v>0.01497704798992</v>
       </c>
       <c r="K214" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L214" t="b">
         <v>0</v>
@@ -9444,10 +9444,10 @@
         <v>7</v>
       </c>
       <c r="C215" t="n">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="D215" t="n">
-        <v>1014</v>
+        <v>1005</v>
       </c>
       <c r="E215" t="b">
         <v>1</v>
@@ -9457,19 +9457,19 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025  , 0.02539, 0.025  ]), TrackedArray([0.22979, 0.07604, 0.97442]))</t>
+          <t>(TrackedArray([0.02506, 0.025  , 0.02503]), TrackedArray([0.26975, 0.975  , 0.06549]))</t>
         </is>
       </c>
       <c r="H215" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m709/m709.off</t>
+          <t>testModels/refined_db/7/m707/m707.off</t>
         </is>
       </c>
       <c r="I215" t="n">
-        <v>0.0003573684656633618</v>
+        <v>0.06494472469930278</v>
       </c>
       <c r="J215" t="n">
-        <v>0.009848593029662593</v>
+        <v>0.009405908309349748</v>
       </c>
       <c r="K215" t="b">
         <v>0</v>
@@ -9489,7 +9489,7 @@
         <v>2000</v>
       </c>
       <c r="D216" t="n">
-        <v>1048</v>
+        <v>1032</v>
       </c>
       <c r="E216" t="b">
         <v>1</v>
@@ -9499,19 +9499,19 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.0255 , 0.02814, 0.025  ]), TrackedArray([0.22092, 0.07791, 0.97344]))</t>
+          <t>(TrackedArray([0.02512, 0.025  , 0.025  ]), TrackedArray([0.44415, 0.975  , 0.06419]))</t>
         </is>
       </c>
       <c r="H216" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m710/m710.off</t>
+          <t>testModels/refined_db/7/m708/m708.off</t>
         </is>
       </c>
       <c r="I216" t="n">
-        <v>0.00977703969522959</v>
+        <v>0.004282833850689033</v>
       </c>
       <c r="J216" t="n">
-        <v>0.009225152976660354</v>
+        <v>0.01559969183422879</v>
       </c>
       <c r="K216" t="b">
         <v>0</v>
@@ -9528,10 +9528,10 @@
         <v>7</v>
       </c>
       <c r="C217" t="n">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="D217" t="n">
-        <v>1152</v>
+        <v>1014</v>
       </c>
       <c r="E217" t="b">
         <v>1</v>
@@ -9541,25 +9541,25 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.22872, 0.0556 , 0.97108]))</t>
+          <t>(TrackedArray([0.025  , 0.02539, 0.025  ]), TrackedArray([0.22979, 0.07604, 0.97442]))</t>
         </is>
       </c>
       <c r="H217" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m711/m711.off</t>
+          <t>testModels/refined_db/7/m709/m709.off</t>
         </is>
       </c>
       <c r="I217" t="n">
-        <v>1.872605474088358e-05</v>
+        <v>0.0003573684656633618</v>
       </c>
       <c r="J217" t="n">
-        <v>0.005898091483909225</v>
+        <v>0.009848593029662593</v>
       </c>
       <c r="K217" t="b">
         <v>0</v>
       </c>
       <c r="L217" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="218">
@@ -9573,7 +9573,7 @@
         <v>2000</v>
       </c>
       <c r="D218" t="n">
-        <v>1096</v>
+        <v>1048</v>
       </c>
       <c r="E218" t="b">
         <v>1</v>
@@ -9583,19 +9583,19 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025  , 0.025  , 0.02511]), TrackedArray([0.97497, 0.0565 , 0.2089 ]))</t>
+          <t>(TrackedArray([0.0255 , 0.02814, 0.025  ]), TrackedArray([0.22092, 0.07791, 0.97344]))</t>
         </is>
       </c>
       <c r="H218" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m712/m712.off</t>
+          <t>testModels/refined_db/7/m710/m710.off</t>
         </is>
       </c>
       <c r="I218" t="n">
-        <v>0.0008682165576076732</v>
+        <v>0.00977703969522959</v>
       </c>
       <c r="J218" t="n">
-        <v>0.005499642830204251</v>
+        <v>0.009225152976660354</v>
       </c>
       <c r="K218" t="b">
         <v>0</v>
@@ -9609,13 +9609,13 @@
         <v>217</v>
       </c>
       <c r="B219" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C219" t="n">
-        <v>1958</v>
+        <v>1999</v>
       </c>
       <c r="D219" t="n">
-        <v>1000</v>
+        <v>1152</v>
       </c>
       <c r="E219" t="b">
         <v>1</v>
@@ -9625,25 +9625,25 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.72778, 0.975  , 0.72778]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.22872, 0.0556 , 0.97108]))</t>
         </is>
       </c>
       <c r="H219" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m800/m800.off</t>
+          <t>testModels/refined_db/7/m711/m711.off</t>
         </is>
       </c>
       <c r="I219" t="n">
-        <v>0.00229425835594984</v>
+        <v>1.872605474088358e-05</v>
       </c>
       <c r="J219" t="n">
-        <v>0.4692020714198</v>
+        <v>0.005898091483909225</v>
       </c>
       <c r="K219" t="b">
         <v>0</v>
       </c>
       <c r="L219" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="220">
@@ -9651,13 +9651,13 @@
         <v>218</v>
       </c>
       <c r="B220" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C220" t="n">
         <v>2000</v>
       </c>
       <c r="D220" t="n">
-        <v>1054</v>
+        <v>1096</v>
       </c>
       <c r="E220" t="b">
         <v>1</v>
@@ -9667,19 +9667,19 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.02682, 0.02561, 0.025  ]), TrackedArray([0.46699, 0.975  , 0.54432]))</t>
+          <t>(TrackedArray([0.025  , 0.025  , 0.02511]), TrackedArray([0.97497, 0.0565 , 0.2089 ]))</t>
         </is>
       </c>
       <c r="H220" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m801/m801.off</t>
+          <t>testModels/refined_db/7/m712/m712.off</t>
         </is>
       </c>
       <c r="I220" t="n">
-        <v>0.02356440389067259</v>
+        <v>0.0008682165576076732</v>
       </c>
       <c r="J220" t="n">
-        <v>0.2170203488597468</v>
+        <v>0.005499642830204251</v>
       </c>
       <c r="K220" t="b">
         <v>0</v>
@@ -9696,7 +9696,7 @@
         <v>8</v>
       </c>
       <c r="C221" t="n">
-        <v>1850</v>
+        <v>1958</v>
       </c>
       <c r="D221" t="n">
         <v>1000</v>
@@ -9709,19 +9709,19 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.68578, 0.975  , 0.69614]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.72778, 0.975  , 0.72778]))</t>
         </is>
       </c>
       <c r="H221" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m802/m802.off</t>
+          <t>testModels/refined_db/8/m800/m800.off</t>
         </is>
       </c>
       <c r="I221" t="n">
-        <v>6.509696913035947e-05</v>
+        <v>0.00229425835594984</v>
       </c>
       <c r="J221" t="n">
-        <v>0.4212982889336</v>
+        <v>0.4692020714198</v>
       </c>
       <c r="K221" t="b">
         <v>0</v>
@@ -9741,7 +9741,7 @@
         <v>2000</v>
       </c>
       <c r="D222" t="n">
-        <v>1058</v>
+        <v>1054</v>
       </c>
       <c r="E222" t="b">
         <v>1</v>
@@ -9751,19 +9751,19 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.5701 , 0.975  , 0.60681]))</t>
+          <t>(TrackedArray([0.02682, 0.02561, 0.025  ]), TrackedArray([0.46699, 0.975  , 0.54432]))</t>
         </is>
       </c>
       <c r="H222" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m803/m803.off</t>
+          <t>testModels/refined_db/8/m801/m801.off</t>
         </is>
       </c>
       <c r="I222" t="n">
-        <v>0.0001037527882258007</v>
+        <v>0.02356440389067259</v>
       </c>
       <c r="J222" t="n">
-        <v>0.30128957545635</v>
+        <v>0.2170203488597468</v>
       </c>
       <c r="K222" t="b">
         <v>0</v>
@@ -9780,7 +9780,7 @@
         <v>8</v>
       </c>
       <c r="C223" t="n">
-        <v>1900</v>
+        <v>1850</v>
       </c>
       <c r="D223" t="n">
         <v>1000</v>
@@ -9793,19 +9793,19 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.70218, 0.975  , 0.66904]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.68578, 0.975  , 0.69614]))</t>
         </is>
       </c>
       <c r="H223" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m804/m804.off</t>
+          <t>testModels/refined_db/8/m802/m802.off</t>
         </is>
       </c>
       <c r="I223" t="n">
-        <v>0.002552374671082288</v>
+        <v>6.509696913035947e-05</v>
       </c>
       <c r="J223" t="n">
-        <v>0.4143275475168</v>
+        <v>0.4212982889336</v>
       </c>
       <c r="K223" t="b">
         <v>0</v>
@@ -9822,10 +9822,10 @@
         <v>8</v>
       </c>
       <c r="C224" t="n">
-        <v>1992</v>
+        <v>2000</v>
       </c>
       <c r="D224" t="n">
-        <v>1000</v>
+        <v>1058</v>
       </c>
       <c r="E224" t="b">
         <v>1</v>
@@ -9835,19 +9835,19 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.72976, 0.975  , 0.72976]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.5701 , 0.975  , 0.60681]))</t>
         </is>
       </c>
       <c r="H224" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m805/m805.off</t>
+          <t>testModels/refined_db/8/m803/m803.off</t>
         </is>
       </c>
       <c r="I224" t="n">
-        <v>0.0003921532034501675</v>
+        <v>0.0001037527882258007</v>
       </c>
       <c r="J224" t="n">
-        <v>0.4718550028118</v>
+        <v>0.30128957545635</v>
       </c>
       <c r="K224" t="b">
         <v>0</v>
@@ -9864,7 +9864,7 @@
         <v>8</v>
       </c>
       <c r="C225" t="n">
-        <v>1968</v>
+        <v>1900</v>
       </c>
       <c r="D225" t="n">
         <v>1000</v>
@@ -9877,19 +9877,19 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.35829, 0.975  , 0.41154]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.70218, 0.975  , 0.66904]))</t>
         </is>
       </c>
       <c r="H225" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m806/m806.off</t>
+          <t>testModels/refined_db/8/m804/m804.off</t>
         </is>
       </c>
       <c r="I225" t="n">
-        <v>6.230126594257498e-05</v>
+        <v>0.002552374671082288</v>
       </c>
       <c r="J225" t="n">
-        <v>0.12238963667975</v>
+        <v>0.4143275475168</v>
       </c>
       <c r="K225" t="b">
         <v>0</v>
@@ -9906,7 +9906,7 @@
         <v>8</v>
       </c>
       <c r="C226" t="n">
-        <v>1976</v>
+        <v>1992</v>
       </c>
       <c r="D226" t="n">
         <v>1000</v>
@@ -9919,19 +9919,19 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.405  , 0.975  , 0.40384]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.72976, 0.975  , 0.72976]))</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m807/m807.off</t>
+          <t>testModels/refined_db/8/m805/m805.off</t>
         </is>
       </c>
       <c r="I226" t="n">
-        <v>0.001213741904721069</v>
+        <v>0.0003921532034501675</v>
       </c>
       <c r="J226" t="n">
-        <v>0.136760518</v>
+        <v>0.4718550028118</v>
       </c>
       <c r="K226" t="b">
         <v>0</v>
@@ -9948,7 +9948,7 @@
         <v>8</v>
       </c>
       <c r="C227" t="n">
-        <v>1660</v>
+        <v>1968</v>
       </c>
       <c r="D227" t="n">
         <v>1000</v>
@@ -9961,19 +9961,19 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.55085, 0.975  , 0.62458]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.35829, 0.975  , 0.41154]))</t>
         </is>
       </c>
       <c r="H227" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m808/m808.off</t>
+          <t>testModels/refined_db/8/m806/m806.off</t>
         </is>
       </c>
       <c r="I227" t="n">
-        <v>0.0005334409098800224</v>
+        <v>6.230126594257498e-05</v>
       </c>
       <c r="J227" t="n">
-        <v>0.29952589509265</v>
+        <v>0.12238963667975</v>
       </c>
       <c r="K227" t="b">
         <v>0</v>
@@ -9990,7 +9990,7 @@
         <v>8</v>
       </c>
       <c r="C228" t="n">
-        <v>1940</v>
+        <v>1976</v>
       </c>
       <c r="D228" t="n">
         <v>1000</v>
@@ -10003,19 +10003,19 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.24254, 0.975  , 0.22572]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.405  , 0.975  , 0.40384]))</t>
         </is>
       </c>
       <c r="H228" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m809/m809.off</t>
+          <t>testModels/refined_db/8/m807/m807.off</t>
         </is>
       </c>
       <c r="I228" t="n">
-        <v>0.001741736583522547</v>
+        <v>0.001213741904721069</v>
       </c>
       <c r="J228" t="n">
-        <v>0.04148136539820001</v>
+        <v>0.136760518</v>
       </c>
       <c r="K228" t="b">
         <v>0</v>
@@ -10032,7 +10032,7 @@
         <v>8</v>
       </c>
       <c r="C229" t="n">
-        <v>1944</v>
+        <v>1660</v>
       </c>
       <c r="D229" t="n">
         <v>1000</v>
@@ -10045,19 +10045,19 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.38296, 0.975  , 0.3995 ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.55085, 0.975  , 0.62458]))</t>
         </is>
       </c>
       <c r="H229" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m810/m810.off</t>
+          <t>testModels/refined_db/8/m808/m808.off</t>
         </is>
       </c>
       <c r="I229" t="n">
-        <v>0.0005863661447857373</v>
+        <v>0.0005334409098800224</v>
       </c>
       <c r="J229" t="n">
-        <v>0.1273507914384</v>
+        <v>0.29952589509265</v>
       </c>
       <c r="K229" t="b">
         <v>0</v>
@@ -10074,10 +10074,10 @@
         <v>8</v>
       </c>
       <c r="C230" t="n">
-        <v>1920</v>
+        <v>1940</v>
       </c>
       <c r="D230" t="n">
-        <v>964</v>
+        <v>1000</v>
       </c>
       <c r="E230" t="b">
         <v>1</v>
@@ -10087,19 +10087,19 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.53825, 0.975  , 0.55673]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.24254, 0.975  , 0.22572]))</t>
         </is>
       </c>
       <c r="H230" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m811/m811.off</t>
+          <t>testModels/refined_db/8/m809/m809.off</t>
         </is>
       </c>
       <c r="I230" t="n">
-        <v>0.0003918203221181705</v>
+        <v>0.001741736583522547</v>
       </c>
       <c r="J230" t="n">
-        <v>0.2592673744301999</v>
+        <v>0.04148136539820001</v>
       </c>
       <c r="K230" t="b">
         <v>0</v>
@@ -10116,10 +10116,10 @@
         <v>8</v>
       </c>
       <c r="C231" t="n">
-        <v>1920</v>
+        <v>1944</v>
       </c>
       <c r="D231" t="n">
-        <v>976</v>
+        <v>1000</v>
       </c>
       <c r="E231" t="b">
         <v>1</v>
@@ -10129,19 +10129,19 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.46015, 0.975  , 0.47582]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.38296, 0.975  , 0.3995 ]))</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m812/m812.off</t>
+          <t>testModels/refined_db/8/m810/m810.off</t>
         </is>
       </c>
       <c r="I231" t="n">
-        <v>9.637779485730415e-05</v>
+        <v>0.0005863661447857373</v>
       </c>
       <c r="J231" t="n">
-        <v>0.18636813187305</v>
+        <v>0.1273507914384</v>
       </c>
       <c r="K231" t="b">
         <v>0</v>
@@ -10155,13 +10155,13 @@
         <v>230</v>
       </c>
       <c r="B232" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C232" t="n">
-        <v>1772</v>
+        <v>1920</v>
       </c>
       <c r="D232" t="n">
-        <v>1000</v>
+        <v>964</v>
       </c>
       <c r="E232" t="b">
         <v>1</v>
@@ -10171,19 +10171,19 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.61843, 0.38125]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.53825, 0.975  , 0.55673]))</t>
         </is>
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m900/m900.off</t>
+          <t>testModels/refined_db/8/m811/m811.off</t>
         </is>
       </c>
       <c r="I232" t="n">
-        <v>0.0009292084722142014</v>
+        <v>0.0003918203221181705</v>
       </c>
       <c r="J232" t="n">
-        <v>0.2008387393843999</v>
+        <v>0.2592673744301999</v>
       </c>
       <c r="K232" t="b">
         <v>0</v>
@@ -10197,13 +10197,13 @@
         <v>231</v>
       </c>
       <c r="B233" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C233" t="n">
-        <v>1980</v>
+        <v>1920</v>
       </c>
       <c r="D233" t="n">
-        <v>1000</v>
+        <v>976</v>
       </c>
       <c r="E233" t="b">
         <v>1</v>
@@ -10213,19 +10213,19 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.74465, 0.75526]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.46015, 0.975  , 0.47582]))</t>
         </is>
       </c>
       <c r="H233" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m901/m901.off</t>
+          <t>testModels/refined_db/8/m812/m812.off</t>
         </is>
       </c>
       <c r="I233" t="n">
-        <v>0.0008655712038301684</v>
+        <v>9.637779485730415e-05</v>
       </c>
       <c r="J233" t="n">
-        <v>0.4992543045531</v>
+        <v>0.18636813187305</v>
       </c>
       <c r="K233" t="b">
         <v>0</v>
@@ -10242,7 +10242,7 @@
         <v>9</v>
       </c>
       <c r="C234" t="n">
-        <v>1976</v>
+        <v>1772</v>
       </c>
       <c r="D234" t="n">
         <v>1000</v>
@@ -10255,19 +10255,19 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.59618, 0.43685]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.61843, 0.38125]))</t>
         </is>
       </c>
       <c r="H234" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m902/m902.off</t>
+          <t>testModels/refined_db/9/m900/m900.off</t>
         </is>
       </c>
       <c r="I234" t="n">
-        <v>0.002001445678988587</v>
+        <v>0.0009292084722142014</v>
       </c>
       <c r="J234" t="n">
-        <v>0.2234783074855499</v>
+        <v>0.2008387393843999</v>
       </c>
       <c r="K234" t="b">
         <v>0</v>
@@ -10297,19 +10297,19 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.25027, 0.23617]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.74465, 0.75526]))</t>
         </is>
       </c>
       <c r="H235" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m903/m903.off</t>
+          <t>testModels/refined_db/9/m901/m901.off</t>
         </is>
       </c>
       <c r="I235" t="n">
-        <v>0.00108864211424962</v>
+        <v>0.0008655712038301684</v>
       </c>
       <c r="J235" t="n">
-        <v>0.0451911105855</v>
+        <v>0.4992543045531</v>
       </c>
       <c r="K235" t="b">
         <v>0</v>
@@ -10326,7 +10326,7 @@
         <v>9</v>
       </c>
       <c r="C236" t="n">
-        <v>1896</v>
+        <v>1976</v>
       </c>
       <c r="D236" t="n">
         <v>1000</v>
@@ -10339,19 +10339,19 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.40595, 0.975  , 0.40595]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.59618, 0.43685]))</t>
         </is>
       </c>
       <c r="H236" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m904/m904.off</t>
+          <t>testModels/refined_db/9/m902/m902.off</t>
         </is>
       </c>
       <c r="I236" t="n">
-        <v>9.153055386713679e-05</v>
+        <v>0.002001445678988587</v>
       </c>
       <c r="J236" t="n">
-        <v>0.13786748118095</v>
+        <v>0.2234783074855499</v>
       </c>
       <c r="K236" t="b">
         <v>0</v>
@@ -10368,10 +10368,10 @@
         <v>9</v>
       </c>
       <c r="C237" t="n">
-        <v>1972</v>
+        <v>1980</v>
       </c>
       <c r="D237" t="n">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E237" t="b">
         <v>1</v>
@@ -10381,19 +10381,19 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.84105, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.25027, 0.23617]))</t>
         </is>
       </c>
       <c r="H237" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m905/m905.off</t>
+          <t>testModels/refined_db/9/m903/m903.off</t>
         </is>
       </c>
       <c r="I237" t="n">
-        <v>0.01783165915719444</v>
+        <v>0.00108864211424962</v>
       </c>
       <c r="J237" t="n">
-        <v>0.7364851249999999</v>
+        <v>0.0451911105855</v>
       </c>
       <c r="K237" t="b">
         <v>0</v>
@@ -10410,7 +10410,7 @@
         <v>9</v>
       </c>
       <c r="C238" t="n">
-        <v>1956</v>
+        <v>1896</v>
       </c>
       <c r="D238" t="n">
         <v>1000</v>
@@ -10423,19 +10423,19 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.73251, 0.35051, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.40595, 0.975  , 0.40595]))</t>
         </is>
       </c>
       <c r="H238" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m906/m906.off</t>
+          <t>testModels/refined_db/9/m904/m904.off</t>
         </is>
       </c>
       <c r="I238" t="n">
-        <v>9.369465416477644e-05</v>
+        <v>9.153055386713679e-05</v>
       </c>
       <c r="J238" t="n">
-        <v>0.2187877917004</v>
+        <v>0.13786748118095</v>
       </c>
       <c r="K238" t="b">
         <v>0</v>
@@ -10452,10 +10452,10 @@
         <v>9</v>
       </c>
       <c r="C239" t="n">
-        <v>1898</v>
+        <v>1972</v>
       </c>
       <c r="D239" t="n">
-        <v>1000</v>
+        <v>995</v>
       </c>
       <c r="E239" t="b">
         <v>1</v>
@@ -10465,19 +10465,19 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.46091, 0.975  , 0.46112]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.84105, 0.975  ]))</t>
         </is>
       </c>
       <c r="H239" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m907/m907.off</t>
+          <t>testModels/refined_db/9/m905/m905.off</t>
         </is>
       </c>
       <c r="I239" t="n">
-        <v>9.091806591361756e-08</v>
+        <v>0.01783165915719444</v>
       </c>
       <c r="J239" t="n">
-        <v>0.1806036165228</v>
+        <v>0.7364851249999999</v>
       </c>
       <c r="K239" t="b">
         <v>0</v>
@@ -10494,7 +10494,7 @@
         <v>9</v>
       </c>
       <c r="C240" t="n">
-        <v>1772</v>
+        <v>1956</v>
       </c>
       <c r="D240" t="n">
         <v>1000</v>
@@ -10507,19 +10507,19 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.38093, 0.5    ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.73251, 0.35051, 0.975  ]))</t>
         </is>
       </c>
       <c r="H240" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m908/m908.off</t>
+          <t>testModels/refined_db/9/m906/m906.off</t>
         </is>
       </c>
       <c r="I240" t="n">
-        <v>0.0006813556252919533</v>
+        <v>9.369465416477644e-05</v>
       </c>
       <c r="J240" t="n">
-        <v>0.1606127350113</v>
+        <v>0.2187877917004</v>
       </c>
       <c r="K240" t="b">
         <v>0</v>
@@ -10536,7 +10536,7 @@
         <v>9</v>
       </c>
       <c r="C241" t="n">
-        <v>1974</v>
+        <v>1898</v>
       </c>
       <c r="D241" t="n">
         <v>1000</v>
@@ -10549,19 +10549,19 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.47863, 0.5    ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.46091, 0.975  , 0.46112]))</t>
         </is>
       </c>
       <c r="H241" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m911/m911.off</t>
+          <t>testModels/refined_db/9/m907/m907.off</t>
         </is>
       </c>
       <c r="I241" t="n">
-        <v>0.004597958658645679</v>
+        <v>9.091806591361756e-08</v>
       </c>
       <c r="J241" t="n">
-        <v>0.20469828125</v>
+        <v>0.1806036165228</v>
       </c>
       <c r="K241" t="b">
         <v>0</v>
@@ -10578,7 +10578,7 @@
         <v>9</v>
       </c>
       <c r="C242" t="n">
-        <v>1988</v>
+        <v>1772</v>
       </c>
       <c r="D242" t="n">
         <v>1000</v>
@@ -10591,24 +10591,150 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.38093, 0.5    ]))</t>
+        </is>
+      </c>
+      <c r="H242" t="inlineStr">
+        <is>
+          <t>testModels/refined_db/9/m908/m908.off</t>
+        </is>
+      </c>
+      <c r="I242" t="n">
+        <v>0.0006813556252919533</v>
+      </c>
+      <c r="J242" t="n">
+        <v>0.1606127350113</v>
+      </c>
+      <c r="K242" t="b">
+        <v>0</v>
+      </c>
+      <c r="L242" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="n">
+        <v>241</v>
+      </c>
+      <c r="B243" t="n">
+        <v>9</v>
+      </c>
+      <c r="C243" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D243" t="n">
+        <v>1010</v>
+      </c>
+      <c r="E243" t="b">
+        <v>1</v>
+      </c>
+      <c r="F243" t="b">
+        <v>0</v>
+      </c>
+      <c r="G243" t="inlineStr">
+        <is>
+          <t>(TrackedArray([0.025  , 0.02623, 0.025  ]), TrackedArray([0.70357, 0.44378, 0.975  ]))</t>
+        </is>
+      </c>
+      <c r="H243" t="inlineStr">
+        <is>
+          <t>testModels/refined_db/9/m909/m909.off</t>
+        </is>
+      </c>
+      <c r="I243" t="n">
+        <v>0.1286547542692651</v>
+      </c>
+      <c r="J243" t="n">
+        <v>0.2691700682120299</v>
+      </c>
+      <c r="K243" t="b">
+        <v>0</v>
+      </c>
+      <c r="L243" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="1" t="n">
+        <v>242</v>
+      </c>
+      <c r="B244" t="n">
+        <v>9</v>
+      </c>
+      <c r="C244" t="n">
+        <v>1974</v>
+      </c>
+      <c r="D244" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E244" t="b">
+        <v>1</v>
+      </c>
+      <c r="F244" t="b">
+        <v>0</v>
+      </c>
+      <c r="G244" t="inlineStr">
+        <is>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.47863, 0.5    ]))</t>
+        </is>
+      </c>
+      <c r="H244" t="inlineStr">
+        <is>
+          <t>testModels/refined_db/9/m911/m911.off</t>
+        </is>
+      </c>
+      <c r="I244" t="n">
+        <v>0.004597958658645679</v>
+      </c>
+      <c r="J244" t="n">
+        <v>0.20469828125</v>
+      </c>
+      <c r="K244" t="b">
+        <v>0</v>
+      </c>
+      <c r="L244" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="1" t="n">
+        <v>243</v>
+      </c>
+      <c r="B245" t="n">
+        <v>9</v>
+      </c>
+      <c r="C245" t="n">
+        <v>1988</v>
+      </c>
+      <c r="D245" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E245" t="b">
+        <v>1</v>
+      </c>
+      <c r="F245" t="b">
+        <v>0</v>
+      </c>
+      <c r="G245" t="inlineStr">
+        <is>
           <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975, 0.5  , 0.5  ]))</t>
         </is>
       </c>
-      <c r="H242" t="inlineStr">
+      <c r="H245" t="inlineStr">
         <is>
           <t>testModels/refined_db/9/m912/m912.off</t>
         </is>
       </c>
-      <c r="I242" t="n">
+      <c r="I245" t="n">
         <v>0.001119938230630489</v>
       </c>
-      <c r="J242" t="n">
+      <c r="J245" t="n">
         <v>0.21434375</v>
       </c>
-      <c r="K242" t="b">
-        <v>0</v>
-      </c>
-      <c r="L242" t="b">
+      <c r="K245" t="b">
+        <v>0</v>
+      </c>
+      <c r="L245" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed barycentre and scaling function
</commit_message>
<xml_diff>
--- a/features/refined.xlsx
+++ b/features/refined.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L242"/>
+  <dimension ref="A1:L245"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7935,7 +7935,7 @@
         <v>2000</v>
       </c>
       <c r="D179" t="n">
-        <v>1472</v>
+        <v>1179</v>
       </c>
       <c r="E179" t="b">
         <v>1</v>
@@ -7945,19 +7945,19 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.12811, 0.51158]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.44198, 0.94572]))</t>
         </is>
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t>testModels/refined_db/4/m412/m412.off</t>
+          <t>testModels/refined_db/4/m410/m410.off</t>
         </is>
       </c>
       <c r="I179" t="n">
-        <v>0.02426980825759749</v>
+        <v>0.4426165134704702</v>
       </c>
       <c r="J179" t="n">
-        <v>0.04766319038249999</v>
+        <v>0.36472700513595</v>
       </c>
       <c r="K179" t="b">
         <v>0</v>
@@ -7971,13 +7971,13 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C180" t="n">
-        <v>1996</v>
+        <v>2000</v>
       </c>
       <c r="D180" t="n">
-        <v>1000</v>
+        <v>1009</v>
       </c>
       <c r="E180" t="b">
         <v>1</v>
@@ -7987,19 +7987,19 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.95964, 0.89686, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.70357, 0.45049]))</t>
         </is>
       </c>
       <c r="H180" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m500/m500.off</t>
+          <t>testModels/refined_db/4/m411/m411.off</t>
         </is>
       </c>
       <c r="I180" t="n">
-        <v>0.0006964191987781477</v>
+        <v>0.356823088341781</v>
       </c>
       <c r="J180" t="n">
-        <v>0.774133244696</v>
+        <v>0.2742882714080499</v>
       </c>
       <c r="K180" t="b">
         <v>0</v>
@@ -8013,13 +8013,13 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C181" t="n">
         <v>2000</v>
       </c>
       <c r="D181" t="n">
-        <v>1072</v>
+        <v>1472</v>
       </c>
       <c r="E181" t="b">
         <v>1</v>
@@ -8029,25 +8029,25 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.67754, 0.975  , 0.67754]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.12811, 0.51158]))</t>
         </is>
       </c>
       <c r="H181" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m501/m501.off</t>
+          <t>testModels/refined_db/4/m412/m412.off</t>
         </is>
       </c>
       <c r="I181" t="n">
-        <v>0.0001625845650226333</v>
+        <v>0.02426980825759749</v>
       </c>
       <c r="J181" t="n">
-        <v>0.4045155493718</v>
+        <v>0.04766319038249999</v>
       </c>
       <c r="K181" t="b">
         <v>0</v>
       </c>
       <c r="L181" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182">
@@ -8071,19 +8071,19 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.67501, 0.975  , 0.67501]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.95964, 0.89686, 0.975  ]))</t>
         </is>
       </c>
       <c r="H182" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m502/m502.off</t>
+          <t>testModels/refined_db/5/m500/m500.off</t>
         </is>
       </c>
       <c r="I182" t="n">
-        <v>0.002764792734748884</v>
+        <v>0.0006964191987781477</v>
       </c>
       <c r="J182" t="n">
-        <v>0.4013836450465499</v>
+        <v>0.774133244696</v>
       </c>
       <c r="K182" t="b">
         <v>0</v>
@@ -8100,10 +8100,10 @@
         <v>5</v>
       </c>
       <c r="C183" t="n">
-        <v>1952</v>
+        <v>2000</v>
       </c>
       <c r="D183" t="n">
-        <v>1000</v>
+        <v>1072</v>
       </c>
       <c r="E183" t="b">
         <v>1</v>
@@ -8113,19 +8113,19 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.8853, 0.975 , 0.5708]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.67754, 0.975  , 0.67754]))</t>
         </is>
       </c>
       <c r="H183" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m503/m503.off</t>
+          <t>testModels/refined_db/5/m501/m501.off</t>
         </is>
       </c>
       <c r="I183" t="n">
-        <v>0.002016172263500733</v>
+        <v>0.0001625845650226333</v>
       </c>
       <c r="J183" t="n">
-        <v>0.44607162209075</v>
+        <v>0.4045155493718</v>
       </c>
       <c r="K183" t="b">
         <v>0</v>
@@ -8142,7 +8142,7 @@
         <v>5</v>
       </c>
       <c r="C184" t="n">
-        <v>2000</v>
+        <v>1996</v>
       </c>
       <c r="D184" t="n">
         <v>1000</v>
@@ -8155,19 +8155,19 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.73697, 0.77026]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.67501, 0.975  , 0.67501]))</t>
         </is>
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m504/m504.off</t>
+          <t>testModels/refined_db/5/m502/m502.off</t>
         </is>
       </c>
       <c r="I184" t="n">
-        <v>2.155574185068136e-05</v>
+        <v>0.002764792734748884</v>
       </c>
       <c r="J184" t="n">
-        <v>0.50407117646765</v>
+        <v>0.4013836450465499</v>
       </c>
       <c r="K184" t="b">
         <v>0</v>
@@ -8184,10 +8184,10 @@
         <v>5</v>
       </c>
       <c r="C185" t="n">
-        <v>2000</v>
+        <v>1952</v>
       </c>
       <c r="D185" t="n">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="E185" t="b">
         <v>1</v>
@@ -8197,19 +8197,19 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.02521, 0.02544, 0.025  ]), TrackedArray([0.97299, 0.65558, 0.92819]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.8853, 0.975 , 0.5708]))</t>
         </is>
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m505/m505.off</t>
+          <t>testModels/refined_db/5/m503/m503.off</t>
         </is>
       </c>
       <c r="I185" t="n">
-        <v>0.00526397823374702</v>
+        <v>0.002016172263500733</v>
       </c>
       <c r="J185" t="n">
-        <v>0.5394184393397173</v>
+        <v>0.44607162209075</v>
       </c>
       <c r="K185" t="b">
         <v>0</v>
@@ -8229,7 +8229,7 @@
         <v>2000</v>
       </c>
       <c r="D186" t="n">
-        <v>1008</v>
+        <v>1000</v>
       </c>
       <c r="E186" t="b">
         <v>1</v>
@@ -8239,19 +8239,19 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.97449, 0.38986, 0.68268]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.73697, 0.77026]))</t>
         </is>
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m506/m506.off</t>
+          <t>testModels/refined_db/5/m504/m504.off</t>
         </is>
       </c>
       <c r="I186" t="n">
-        <v>0.0003049739221834936</v>
+        <v>2.155574185068136e-05</v>
       </c>
       <c r="J186" t="n">
-        <v>0.2278390717677797</v>
+        <v>0.50407117646765</v>
       </c>
       <c r="K186" t="b">
         <v>0</v>
@@ -8281,19 +8281,19 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025  , 0.02504, 0.025  ]), TrackedArray([0.975  , 0.69504, 0.67724]))</t>
+          <t>(TrackedArray([0.02521, 0.02544, 0.025  ]), TrackedArray([0.97299, 0.65558, 0.92819]))</t>
         </is>
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m507/m507.off</t>
+          <t>testModels/refined_db/5/m505/m505.off</t>
         </is>
       </c>
       <c r="I187" t="n">
-        <v>0.0004915109394796224</v>
+        <v>0.00526397823374702</v>
       </c>
       <c r="J187" t="n">
-        <v>0.415150557238935</v>
+        <v>0.5394184393397173</v>
       </c>
       <c r="K187" t="b">
         <v>0</v>
@@ -8310,10 +8310,10 @@
         <v>5</v>
       </c>
       <c r="C188" t="n">
-        <v>1988</v>
+        <v>2000</v>
       </c>
       <c r="D188" t="n">
-        <v>998</v>
+        <v>1008</v>
       </c>
       <c r="E188" t="b">
         <v>1</v>
@@ -8323,19 +8323,19 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.80951, 0.62492]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.97449, 0.38986, 0.68268]))</t>
         </is>
       </c>
       <c r="H188" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m508/m508.off</t>
+          <t>testModels/refined_db/5/m506/m506.off</t>
         </is>
       </c>
       <c r="I188" t="n">
-        <v>2.593299697940728e-05</v>
+        <v>0.0003049739221834936</v>
       </c>
       <c r="J188" t="n">
-        <v>0.4471125239474999</v>
+        <v>0.2278390717677797</v>
       </c>
       <c r="K188" t="b">
         <v>0</v>
@@ -8352,10 +8352,10 @@
         <v>5</v>
       </c>
       <c r="C189" t="n">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="D189" t="n">
-        <v>1002</v>
+        <v>1006</v>
       </c>
       <c r="E189" t="b">
         <v>1</v>
@@ -8365,19 +8365,19 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.0254, 0.025 , 0.025 ]), TrackedArray([0.97303, 0.88927, 0.71394]))</t>
+          <t>(TrackedArray([0.025  , 0.02504, 0.025  ]), TrackedArray([0.975  , 0.69504, 0.67724]))</t>
         </is>
       </c>
       <c r="H189" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m509/m509.off</t>
+          <t>testModels/refined_db/5/m507/m507.off</t>
         </is>
       </c>
       <c r="I189" t="n">
-        <v>0.001541805271098911</v>
+        <v>0.0004915109394796224</v>
       </c>
       <c r="J189" t="n">
-        <v>0.5642497394150771</v>
+        <v>0.415150557238935</v>
       </c>
       <c r="K189" t="b">
         <v>0</v>
@@ -8394,10 +8394,10 @@
         <v>5</v>
       </c>
       <c r="C190" t="n">
-        <v>1999</v>
+        <v>1988</v>
       </c>
       <c r="D190" t="n">
-        <v>1035</v>
+        <v>998</v>
       </c>
       <c r="E190" t="b">
         <v>1</v>
@@ -8407,19 +8407,19 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.60961, 0.97479, 0.52201]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.80951, 0.62492]))</t>
         </is>
       </c>
       <c r="H190" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m510/m510.off</t>
+          <t>testModels/refined_db/5/m508/m508.off</t>
         </is>
       </c>
       <c r="I190" t="n">
-        <v>0.0004058991979104314</v>
+        <v>2.593299697940728e-05</v>
       </c>
       <c r="J190" t="n">
-        <v>0.2759672917384885</v>
+        <v>0.4471125239474999</v>
       </c>
       <c r="K190" t="b">
         <v>0</v>
@@ -8436,10 +8436,10 @@
         <v>5</v>
       </c>
       <c r="C191" t="n">
-        <v>2202</v>
+        <v>1999</v>
       </c>
       <c r="D191" t="n">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E191" t="b">
         <v>1</v>
@@ -8449,19 +8449,19 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.9522 , 0.975  , 0.92067]))</t>
+          <t>(TrackedArray([0.0254, 0.025 , 0.025 ]), TrackedArray([0.97303, 0.88927, 0.71394]))</t>
         </is>
       </c>
       <c r="H191" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m511/m511.off</t>
+          <t>testModels/refined_db/5/m509/m509.off</t>
         </is>
       </c>
       <c r="I191" t="n">
-        <v>0.02789926138668109</v>
+        <v>0.001541805271098911</v>
       </c>
       <c r="J191" t="n">
-        <v>0.7889463070987</v>
+        <v>0.5642497394150771</v>
       </c>
       <c r="K191" t="b">
         <v>0</v>
@@ -8478,10 +8478,10 @@
         <v>5</v>
       </c>
       <c r="C192" t="n">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="D192" t="n">
-        <v>1000</v>
+        <v>1035</v>
       </c>
       <c r="E192" t="b">
         <v>1</v>
@@ -8491,19 +8491,19 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.79759, 0.975  , 0.79759]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.60961, 0.97479, 0.52201]))</t>
         </is>
       </c>
       <c r="H192" t="inlineStr">
         <is>
-          <t>testModels/refined_db/5/m512/m512.off</t>
+          <t>testModels/refined_db/5/m510/m510.off</t>
         </is>
       </c>
       <c r="I192" t="n">
-        <v>0.003047668860747743</v>
+        <v>0.0004058991979104314</v>
       </c>
       <c r="J192" t="n">
-        <v>0.56704613894055</v>
+        <v>0.2759672917384885</v>
       </c>
       <c r="K192" t="b">
         <v>0</v>
@@ -8517,13 +8517,13 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C193" t="n">
-        <v>2000</v>
+        <v>2202</v>
       </c>
       <c r="D193" t="n">
-        <v>1042</v>
+        <v>1000</v>
       </c>
       <c r="E193" t="b">
         <v>1</v>
@@ -8533,19 +8533,19 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.02693, 0.02586, 0.02617]), TrackedArray([0.48928, 0.76584, 0.97387]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.9522 , 0.975  , 0.92067]))</t>
         </is>
       </c>
       <c r="H193" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m600/m600.off</t>
+          <t>testModels/refined_db/5/m511/m511.off</t>
         </is>
       </c>
       <c r="I193" t="n">
-        <v>0.002188264251238722</v>
+        <v>0.02789926138668109</v>
       </c>
       <c r="J193" t="n">
-        <v>0.3242315189462048</v>
+        <v>0.7889463070987</v>
       </c>
       <c r="K193" t="b">
         <v>0</v>
@@ -8559,13 +8559,13 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C194" t="n">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="D194" t="n">
-        <v>1175</v>
+        <v>1000</v>
       </c>
       <c r="E194" t="b">
         <v>1</v>
@@ -8575,25 +8575,25 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.02796, 0.02501, 0.02509]), TrackedArray([0.975  , 0.93453, 0.95622]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.79759, 0.975  , 0.79759]))</t>
         </is>
       </c>
       <c r="H194" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m601/m601.off</t>
+          <t>testModels/refined_db/5/m512/m512.off</t>
         </is>
       </c>
       <c r="I194" t="n">
-        <v>0.001129485291517668</v>
+        <v>0.003047668860747743</v>
       </c>
       <c r="J194" t="n">
-        <v>0.8020325620060286</v>
+        <v>0.56704613894055</v>
       </c>
       <c r="K194" t="b">
         <v>0</v>
       </c>
       <c r="L194" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195">
@@ -8607,7 +8607,7 @@
         <v>2000</v>
       </c>
       <c r="D195" t="n">
-        <v>1008</v>
+        <v>1042</v>
       </c>
       <c r="E195" t="b">
         <v>1</v>
@@ -8617,19 +8617,19 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.02509, 0.025  , 0.025  ]), TrackedArray([0.4276 , 0.975  , 0.59325]))</t>
+          <t>(TrackedArray([0.02693, 0.02586, 0.02617]), TrackedArray([0.48928, 0.76584, 0.97387]))</t>
         </is>
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m602/m602.off</t>
+          <t>testModels/refined_db/6/m600/m600.off</t>
         </is>
       </c>
       <c r="I195" t="n">
-        <v>0.0007723776362440639</v>
+        <v>0.002188264251238722</v>
       </c>
       <c r="J195" t="n">
-        <v>0.217290235051875</v>
+        <v>0.3242315189462048</v>
       </c>
       <c r="K195" t="b">
         <v>0</v>
@@ -8646,10 +8646,10 @@
         <v>6</v>
       </c>
       <c r="C196" t="n">
-        <v>1996</v>
+        <v>1999</v>
       </c>
       <c r="D196" t="n">
-        <v>1000</v>
+        <v>1175</v>
       </c>
       <c r="E196" t="b">
         <v>1</v>
@@ -8659,25 +8659,25 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.58332, 0.84655, 0.975  ]))</t>
+          <t>(TrackedArray([0.02796, 0.02501, 0.02509]), TrackedArray([0.975  , 0.93453, 0.95622]))</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m603/m603.off</t>
+          <t>testModels/refined_db/6/m601/m601.off</t>
         </is>
       </c>
       <c r="I196" t="n">
-        <v>0.000745184319603115</v>
+        <v>0.001129485291517668</v>
       </c>
       <c r="J196" t="n">
-        <v>0.4357544367391</v>
+        <v>0.8020325620060286</v>
       </c>
       <c r="K196" t="b">
         <v>0</v>
       </c>
       <c r="L196" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197">
@@ -8688,10 +8688,10 @@
         <v>6</v>
       </c>
       <c r="C197" t="n">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="D197" t="n">
-        <v>1149</v>
+        <v>1008</v>
       </c>
       <c r="E197" t="b">
         <v>1</v>
@@ -8701,25 +8701,25 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.69906, 0.975  , 0.15606]))</t>
+          <t>(TrackedArray([0.02509, 0.025  , 0.025  ]), TrackedArray([0.4276 , 0.975  , 0.59325]))</t>
         </is>
       </c>
       <c r="H197" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m604/m604.off</t>
+          <t>testModels/refined_db/6/m602/m602.off</t>
         </is>
       </c>
       <c r="I197" t="n">
-        <v>0.02392622713249805</v>
+        <v>0.0007723776362440639</v>
       </c>
       <c r="J197" t="n">
-        <v>0.083922626992</v>
+        <v>0.217290235051875</v>
       </c>
       <c r="K197" t="b">
         <v>0</v>
       </c>
       <c r="L197" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198">
@@ -8730,10 +8730,10 @@
         <v>6</v>
       </c>
       <c r="C198" t="n">
-        <v>2238</v>
+        <v>1996</v>
       </c>
       <c r="D198" t="n">
-        <v>834</v>
+        <v>1000</v>
       </c>
       <c r="E198" t="b">
         <v>1</v>
@@ -8743,22 +8743,22 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.50208, 0.975  , 0.83687]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.58332, 0.84655, 0.975  ]))</t>
         </is>
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m605/m605.off</t>
+          <t>testModels/refined_db/6/m603/m603.off</t>
         </is>
       </c>
       <c r="I198" t="n">
-        <v>0.002287657914562828</v>
+        <v>0.000745184319603115</v>
       </c>
       <c r="J198" t="n">
-        <v>0.36795691912105</v>
+        <v>0.4357544367391</v>
       </c>
       <c r="K198" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L198" t="b">
         <v>0</v>
@@ -8772,10 +8772,10 @@
         <v>6</v>
       </c>
       <c r="C199" t="n">
-        <v>1971</v>
+        <v>1999</v>
       </c>
       <c r="D199" t="n">
-        <v>1000</v>
+        <v>1149</v>
       </c>
       <c r="E199" t="b">
         <v>1</v>
@@ -8785,25 +8785,25 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.83864, 0.975  , 0.45899]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.69906, 0.975  , 0.15606]))</t>
         </is>
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m606/m606.off</t>
+          <t>testModels/refined_db/6/m604/m604.off</t>
         </is>
       </c>
       <c r="I199" t="n">
-        <v>0.01730747197990135</v>
+        <v>0.02392622713249805</v>
       </c>
       <c r="J199" t="n">
-        <v>0.3354520743954</v>
+        <v>0.083922626992</v>
       </c>
       <c r="K199" t="b">
         <v>0</v>
       </c>
       <c r="L199" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200">
@@ -8814,10 +8814,10 @@
         <v>6</v>
       </c>
       <c r="C200" t="n">
-        <v>1709</v>
+        <v>2238</v>
       </c>
       <c r="D200" t="n">
-        <v>901</v>
+        <v>834</v>
       </c>
       <c r="E200" t="b">
         <v>1</v>
@@ -8827,22 +8827,22 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.34539, 0.975  , 0.84361]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.50208, 0.975  , 0.83687]))</t>
         </is>
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m607/m607.off</t>
+          <t>testModels/refined_db/6/m605/m605.off</t>
         </is>
       </c>
       <c r="I200" t="n">
-        <v>1.595780916046108e-05</v>
+        <v>0.002287657914562828</v>
       </c>
       <c r="J200" t="n">
-        <v>0.2491597883831999</v>
+        <v>0.36795691912105</v>
       </c>
       <c r="K200" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L200" t="b">
         <v>0</v>
@@ -8856,7 +8856,7 @@
         <v>6</v>
       </c>
       <c r="C201" t="n">
-        <v>1916</v>
+        <v>1971</v>
       </c>
       <c r="D201" t="n">
         <v>1000</v>
@@ -8869,19 +8869,19 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.75998, 0.90819, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.83864, 0.975  , 0.45899]))</t>
         </is>
       </c>
       <c r="H201" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m608/m608.off</t>
+          <t>testModels/refined_db/6/m606/m606.off</t>
         </is>
       </c>
       <c r="I201" t="n">
-        <v>8.632235975886356e-05</v>
+        <v>0.01730747197990135</v>
       </c>
       <c r="J201" t="n">
-        <v>0.6166739930119999</v>
+        <v>0.3354520743954</v>
       </c>
       <c r="K201" t="b">
         <v>0</v>
@@ -8898,10 +8898,10 @@
         <v>6</v>
       </c>
       <c r="C202" t="n">
-        <v>2000</v>
+        <v>1709</v>
       </c>
       <c r="D202" t="n">
-        <v>1020</v>
+        <v>901</v>
       </c>
       <c r="E202" t="b">
         <v>1</v>
@@ -8911,19 +8911,19 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.21256, 0.72068, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.34539, 0.975  , 0.84361]))</t>
         </is>
       </c>
       <c r="H202" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m609/m609.off</t>
+          <t>testModels/refined_db/6/m607/m607.off</t>
         </is>
       </c>
       <c r="I202" t="n">
-        <v>0.0003560311298754342</v>
+        <v>1.595780916046108e-05</v>
       </c>
       <c r="J202" t="n">
-        <v>0.1239595846008</v>
+        <v>0.2491597883831999</v>
       </c>
       <c r="K202" t="b">
         <v>0</v>
@@ -8940,10 +8940,10 @@
         <v>6</v>
       </c>
       <c r="C203" t="n">
-        <v>2000</v>
+        <v>1916</v>
       </c>
       <c r="D203" t="n">
-        <v>1016</v>
+        <v>1000</v>
       </c>
       <c r="E203" t="b">
         <v>1</v>
@@ -8953,19 +8953,19 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.6368 , 0.55179]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.75998, 0.90819, 0.975  ]))</t>
         </is>
       </c>
       <c r="H203" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m610/m610.off</t>
+          <t>testModels/refined_db/6/m608/m608.off</t>
         </is>
       </c>
       <c r="I203" t="n">
-        <v>1.331384143935641e-05</v>
+        <v>8.632235975886356e-05</v>
       </c>
       <c r="J203" t="n">
-        <v>0.3061758177928125</v>
+        <v>0.6166739930119999</v>
       </c>
       <c r="K203" t="b">
         <v>0</v>
@@ -8982,10 +8982,10 @@
         <v>6</v>
       </c>
       <c r="C204" t="n">
-        <v>2026</v>
+        <v>2000</v>
       </c>
       <c r="D204" t="n">
-        <v>778</v>
+        <v>1020</v>
       </c>
       <c r="E204" t="b">
         <v>1</v>
@@ -8995,22 +8995,22 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.84401, 0.975  , 0.45893]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.21256, 0.72068, 0.975  ]))</t>
         </is>
       </c>
       <c r="H204" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m611/m611.off</t>
+          <t>testModels/refined_db/6/m609/m609.off</t>
         </is>
       </c>
       <c r="I204" t="n">
-        <v>0.006340770550030407</v>
+        <v>0.0003560311298754342</v>
       </c>
       <c r="J204" t="n">
-        <v>0.337626976131</v>
+        <v>0.1239595846008</v>
       </c>
       <c r="K204" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L204" t="b">
         <v>0</v>
@@ -9024,10 +9024,10 @@
         <v>6</v>
       </c>
       <c r="C205" t="n">
-        <v>2232</v>
+        <v>2000</v>
       </c>
       <c r="D205" t="n">
-        <v>948</v>
+        <v>1016</v>
       </c>
       <c r="E205" t="b">
         <v>1</v>
@@ -9037,19 +9037,19 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.75993, 0.90811, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.6368 , 0.55179]))</t>
         </is>
       </c>
       <c r="H205" t="inlineStr">
         <is>
-          <t>testModels/refined_db/6/m612/m612.off</t>
+          <t>testModels/refined_db/6/m610/m610.off</t>
         </is>
       </c>
       <c r="I205" t="n">
-        <v>0.0001209419976838267</v>
+        <v>1.331384143935641e-05</v>
       </c>
       <c r="J205" t="n">
-        <v>0.6165689174602</v>
+        <v>0.3061758177928125</v>
       </c>
       <c r="K205" t="b">
         <v>0</v>
@@ -9063,13 +9063,13 @@
         <v>204</v>
       </c>
       <c r="B206" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C206" t="n">
-        <v>1904</v>
+        <v>2026</v>
       </c>
       <c r="D206" t="n">
-        <v>1000</v>
+        <v>778</v>
       </c>
       <c r="E206" t="b">
         <v>1</v>
@@ -9079,22 +9079,22 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.41837, 0.975  , 0.09773]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.84401, 0.975  , 0.45893]))</t>
         </is>
       </c>
       <c r="H206" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m700/m700.off</t>
+          <t>testModels/refined_db/6/m611/m611.off</t>
         </is>
       </c>
       <c r="I206" t="n">
-        <v>0.001634965579034274</v>
+        <v>0.006340770550030407</v>
       </c>
       <c r="J206" t="n">
-        <v>0.027180761887565</v>
+        <v>0.337626976131</v>
       </c>
       <c r="K206" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L206" t="b">
         <v>0</v>
@@ -9105,13 +9105,13 @@
         <v>205</v>
       </c>
       <c r="B207" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C207" t="n">
-        <v>1900</v>
+        <v>2232</v>
       </c>
       <c r="D207" t="n">
-        <v>960</v>
+        <v>948</v>
       </c>
       <c r="E207" t="b">
         <v>1</v>
@@ -9121,19 +9121,19 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.04405, 0.30701, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.75993, 0.90811, 0.975  ]))</t>
         </is>
       </c>
       <c r="H207" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m701/m701.off</t>
+          <t>testModels/refined_db/6/m612/m612.off</t>
         </is>
       </c>
       <c r="I207" t="n">
-        <v>0.0005984744284004732</v>
+        <v>0.0001209419976838267</v>
       </c>
       <c r="J207" t="n">
-        <v>0.005102765082699999</v>
+        <v>0.6165689174602</v>
       </c>
       <c r="K207" t="b">
         <v>0</v>
@@ -9150,10 +9150,10 @@
         <v>7</v>
       </c>
       <c r="C208" t="n">
-        <v>2000</v>
+        <v>1904</v>
       </c>
       <c r="D208" t="n">
-        <v>1005</v>
+        <v>1000</v>
       </c>
       <c r="E208" t="b">
         <v>1</v>
@@ -9163,19 +9163,19 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.12358, 0.12358, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.41837, 0.975  , 0.09773]))</t>
         </is>
       </c>
       <c r="H208" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m702/m702.off</t>
+          <t>testModels/refined_db/7/m700/m700.off</t>
         </is>
       </c>
       <c r="I208" t="n">
-        <v>0.0002847790346095218</v>
+        <v>0.001634965579034274</v>
       </c>
       <c r="J208" t="n">
-        <v>0.0092317409798</v>
+        <v>0.027180761887565</v>
       </c>
       <c r="K208" t="b">
         <v>0</v>
@@ -9192,10 +9192,10 @@
         <v>7</v>
       </c>
       <c r="C209" t="n">
-        <v>1924</v>
+        <v>1900</v>
       </c>
       <c r="D209" t="n">
-        <v>1000</v>
+        <v>960</v>
       </c>
       <c r="E209" t="b">
         <v>1</v>
@@ -9205,19 +9205,19 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.05076, 0.12084, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.04405, 0.30701, 0.975  ]))</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m703/m703.off</t>
+          <t>testModels/refined_db/7/m701/m701.off</t>
         </is>
       </c>
       <c r="I209" t="n">
-        <v>0.0001905921691495498</v>
+        <v>0.0005984744284004732</v>
       </c>
       <c r="J209" t="n">
-        <v>0.002345430056895</v>
+        <v>0.005102765082699999</v>
       </c>
       <c r="K209" t="b">
         <v>0</v>
@@ -9234,10 +9234,10 @@
         <v>7</v>
       </c>
       <c r="C210" t="n">
-        <v>1996</v>
+        <v>2000</v>
       </c>
       <c r="D210" t="n">
-        <v>1000</v>
+        <v>1005</v>
       </c>
       <c r="E210" t="b">
         <v>1</v>
@@ -9247,19 +9247,19 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.05493, 0.08613, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.12358, 0.12358, 0.975  ]))</t>
         </is>
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m704/m704.off</t>
+          <t>testModels/refined_db/7/m702/m702.off</t>
         </is>
       </c>
       <c r="I210" t="n">
-        <v>9.025291300841998e-05</v>
+        <v>0.0002847790346095218</v>
       </c>
       <c r="J210" t="n">
-        <v>0.001738359126875</v>
+        <v>0.0092317409798</v>
       </c>
       <c r="K210" t="b">
         <v>0</v>
@@ -9276,10 +9276,10 @@
         <v>7</v>
       </c>
       <c r="C211" t="n">
-        <v>2000</v>
+        <v>1924</v>
       </c>
       <c r="D211" t="n">
-        <v>1028</v>
+        <v>1000</v>
       </c>
       <c r="E211" t="b">
         <v>1</v>
@@ -9289,19 +9289,19 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.02655, 0.025  , 0.02525]), TrackedArray([0.46452, 0.975  , 0.09452]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.05076, 0.12084, 0.975  ]))</t>
         </is>
       </c>
       <c r="H211" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m705/m705.off</t>
+          <t>testModels/refined_db/7/m703/m703.off</t>
         </is>
       </c>
       <c r="I211" t="n">
-        <v>0.0005383789458012969</v>
+        <v>0.0001905921691495498</v>
       </c>
       <c r="J211" t="n">
-        <v>0.02882194424788575</v>
+        <v>0.002345430056895</v>
       </c>
       <c r="K211" t="b">
         <v>0</v>
@@ -9318,10 +9318,10 @@
         <v>7</v>
       </c>
       <c r="C212" t="n">
-        <v>1999</v>
+        <v>1996</v>
       </c>
       <c r="D212" t="n">
-        <v>802</v>
+        <v>1000</v>
       </c>
       <c r="E212" t="b">
         <v>1</v>
@@ -9331,22 +9331,22 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025 , 0.025 , 0.0252]), TrackedArray([0.28441, 0.975  , 0.08598]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.05493, 0.08613, 0.975  ]))</t>
         </is>
       </c>
       <c r="H212" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m706/m706.off</t>
+          <t>testModels/refined_db/7/m704/m704.off</t>
         </is>
       </c>
       <c r="I212" t="n">
-        <v>0.000843582869486666</v>
+        <v>9.025291300841998e-05</v>
       </c>
       <c r="J212" t="n">
-        <v>0.01497704798992</v>
+        <v>0.001738359126875</v>
       </c>
       <c r="K212" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L212" t="b">
         <v>0</v>
@@ -9360,10 +9360,10 @@
         <v>7</v>
       </c>
       <c r="C213" t="n">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="D213" t="n">
-        <v>1005</v>
+        <v>1028</v>
       </c>
       <c r="E213" t="b">
         <v>1</v>
@@ -9373,19 +9373,19 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.02506, 0.025  , 0.02503]), TrackedArray([0.26975, 0.975  , 0.06549]))</t>
+          <t>(TrackedArray([0.02655, 0.025  , 0.02525]), TrackedArray([0.46452, 0.975  , 0.09452]))</t>
         </is>
       </c>
       <c r="H213" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m707/m707.off</t>
+          <t>testModels/refined_db/7/m705/m705.off</t>
         </is>
       </c>
       <c r="I213" t="n">
-        <v>0.06494472469930278</v>
+        <v>0.0005383789458012969</v>
       </c>
       <c r="J213" t="n">
-        <v>0.009405908309349748</v>
+        <v>0.02882194424788575</v>
       </c>
       <c r="K213" t="b">
         <v>0</v>
@@ -9402,10 +9402,10 @@
         <v>7</v>
       </c>
       <c r="C214" t="n">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="D214" t="n">
-        <v>1032</v>
+        <v>802</v>
       </c>
       <c r="E214" t="b">
         <v>1</v>
@@ -9415,22 +9415,22 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.02512, 0.025  , 0.025  ]), TrackedArray([0.44415, 0.975  , 0.06419]))</t>
+          <t>(TrackedArray([0.025 , 0.025 , 0.0252]), TrackedArray([0.28441, 0.975  , 0.08598]))</t>
         </is>
       </c>
       <c r="H214" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m708/m708.off</t>
+          <t>testModels/refined_db/7/m706/m706.off</t>
         </is>
       </c>
       <c r="I214" t="n">
-        <v>0.004282833850689033</v>
+        <v>0.000843582869486666</v>
       </c>
       <c r="J214" t="n">
-        <v>0.01559969183422879</v>
+        <v>0.01497704798992</v>
       </c>
       <c r="K214" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L214" t="b">
         <v>0</v>
@@ -9444,10 +9444,10 @@
         <v>7</v>
       </c>
       <c r="C215" t="n">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="D215" t="n">
-        <v>1014</v>
+        <v>1005</v>
       </c>
       <c r="E215" t="b">
         <v>1</v>
@@ -9457,19 +9457,19 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025  , 0.02539, 0.025  ]), TrackedArray([0.22979, 0.07604, 0.97442]))</t>
+          <t>(TrackedArray([0.02506, 0.025  , 0.02503]), TrackedArray([0.26975, 0.975  , 0.06549]))</t>
         </is>
       </c>
       <c r="H215" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m709/m709.off</t>
+          <t>testModels/refined_db/7/m707/m707.off</t>
         </is>
       </c>
       <c r="I215" t="n">
-        <v>0.0003573684656633618</v>
+        <v>0.06494472469930278</v>
       </c>
       <c r="J215" t="n">
-        <v>0.009848593029662593</v>
+        <v>0.009405908309349748</v>
       </c>
       <c r="K215" t="b">
         <v>0</v>
@@ -9489,7 +9489,7 @@
         <v>2000</v>
       </c>
       <c r="D216" t="n">
-        <v>1048</v>
+        <v>1032</v>
       </c>
       <c r="E216" t="b">
         <v>1</v>
@@ -9499,19 +9499,19 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.0255 , 0.02814, 0.025  ]), TrackedArray([0.22092, 0.07791, 0.97344]))</t>
+          <t>(TrackedArray([0.02512, 0.025  , 0.025  ]), TrackedArray([0.44415, 0.975  , 0.06419]))</t>
         </is>
       </c>
       <c r="H216" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m710/m710.off</t>
+          <t>testModels/refined_db/7/m708/m708.off</t>
         </is>
       </c>
       <c r="I216" t="n">
-        <v>0.00977703969522959</v>
+        <v>0.004282833850689033</v>
       </c>
       <c r="J216" t="n">
-        <v>0.009225152976660354</v>
+        <v>0.01559969183422879</v>
       </c>
       <c r="K216" t="b">
         <v>0</v>
@@ -9528,10 +9528,10 @@
         <v>7</v>
       </c>
       <c r="C217" t="n">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="D217" t="n">
-        <v>1152</v>
+        <v>1014</v>
       </c>
       <c r="E217" t="b">
         <v>1</v>
@@ -9541,25 +9541,25 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.22872, 0.0556 , 0.97108]))</t>
+          <t>(TrackedArray([0.025  , 0.02539, 0.025  ]), TrackedArray([0.22979, 0.07604, 0.97442]))</t>
         </is>
       </c>
       <c r="H217" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m711/m711.off</t>
+          <t>testModels/refined_db/7/m709/m709.off</t>
         </is>
       </c>
       <c r="I217" t="n">
-        <v>1.872605474088358e-05</v>
+        <v>0.0003573684656633618</v>
       </c>
       <c r="J217" t="n">
-        <v>0.005898091483909225</v>
+        <v>0.009848593029662593</v>
       </c>
       <c r="K217" t="b">
         <v>0</v>
       </c>
       <c r="L217" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="218">
@@ -9573,7 +9573,7 @@
         <v>2000</v>
       </c>
       <c r="D218" t="n">
-        <v>1096</v>
+        <v>1048</v>
       </c>
       <c r="E218" t="b">
         <v>1</v>
@@ -9583,19 +9583,19 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025  , 0.025  , 0.02511]), TrackedArray([0.97497, 0.0565 , 0.2089 ]))</t>
+          <t>(TrackedArray([0.0255 , 0.02814, 0.025  ]), TrackedArray([0.22092, 0.07791, 0.97344]))</t>
         </is>
       </c>
       <c r="H218" t="inlineStr">
         <is>
-          <t>testModels/refined_db/7/m712/m712.off</t>
+          <t>testModels/refined_db/7/m710/m710.off</t>
         </is>
       </c>
       <c r="I218" t="n">
-        <v>0.0008682165576076732</v>
+        <v>0.00977703969522959</v>
       </c>
       <c r="J218" t="n">
-        <v>0.005499642830204251</v>
+        <v>0.009225152976660354</v>
       </c>
       <c r="K218" t="b">
         <v>0</v>
@@ -9609,13 +9609,13 @@
         <v>217</v>
       </c>
       <c r="B219" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C219" t="n">
-        <v>1958</v>
+        <v>1999</v>
       </c>
       <c r="D219" t="n">
-        <v>1000</v>
+        <v>1152</v>
       </c>
       <c r="E219" t="b">
         <v>1</v>
@@ -9625,25 +9625,25 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.72778, 0.975  , 0.72778]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.22872, 0.0556 , 0.97108]))</t>
         </is>
       </c>
       <c r="H219" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m800/m800.off</t>
+          <t>testModels/refined_db/7/m711/m711.off</t>
         </is>
       </c>
       <c r="I219" t="n">
-        <v>0.00229425835594984</v>
+        <v>1.872605474088358e-05</v>
       </c>
       <c r="J219" t="n">
-        <v>0.4692020714198</v>
+        <v>0.005898091483909225</v>
       </c>
       <c r="K219" t="b">
         <v>0</v>
       </c>
       <c r="L219" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="220">
@@ -9651,13 +9651,13 @@
         <v>218</v>
       </c>
       <c r="B220" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C220" t="n">
         <v>2000</v>
       </c>
       <c r="D220" t="n">
-        <v>1054</v>
+        <v>1096</v>
       </c>
       <c r="E220" t="b">
         <v>1</v>
@@ -9667,19 +9667,19 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.02682, 0.02561, 0.025  ]), TrackedArray([0.46699, 0.975  , 0.54432]))</t>
+          <t>(TrackedArray([0.025  , 0.025  , 0.02511]), TrackedArray([0.97497, 0.0565 , 0.2089 ]))</t>
         </is>
       </c>
       <c r="H220" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m801/m801.off</t>
+          <t>testModels/refined_db/7/m712/m712.off</t>
         </is>
       </c>
       <c r="I220" t="n">
-        <v>0.02356440389067259</v>
+        <v>0.0008682165576076732</v>
       </c>
       <c r="J220" t="n">
-        <v>0.2170203488597468</v>
+        <v>0.005499642830204251</v>
       </c>
       <c r="K220" t="b">
         <v>0</v>
@@ -9696,7 +9696,7 @@
         <v>8</v>
       </c>
       <c r="C221" t="n">
-        <v>1850</v>
+        <v>1958</v>
       </c>
       <c r="D221" t="n">
         <v>1000</v>
@@ -9709,19 +9709,19 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.68578, 0.975  , 0.69614]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.72778, 0.975  , 0.72778]))</t>
         </is>
       </c>
       <c r="H221" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m802/m802.off</t>
+          <t>testModels/refined_db/8/m800/m800.off</t>
         </is>
       </c>
       <c r="I221" t="n">
-        <v>6.509696913035947e-05</v>
+        <v>0.00229425835594984</v>
       </c>
       <c r="J221" t="n">
-        <v>0.4212982889336</v>
+        <v>0.4692020714198</v>
       </c>
       <c r="K221" t="b">
         <v>0</v>
@@ -9741,7 +9741,7 @@
         <v>2000</v>
       </c>
       <c r="D222" t="n">
-        <v>1058</v>
+        <v>1054</v>
       </c>
       <c r="E222" t="b">
         <v>1</v>
@@ -9751,19 +9751,19 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.5701 , 0.975  , 0.60681]))</t>
+          <t>(TrackedArray([0.02682, 0.02561, 0.025  ]), TrackedArray([0.46699, 0.975  , 0.54432]))</t>
         </is>
       </c>
       <c r="H222" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m803/m803.off</t>
+          <t>testModels/refined_db/8/m801/m801.off</t>
         </is>
       </c>
       <c r="I222" t="n">
-        <v>0.0001037527882258007</v>
+        <v>0.02356440389067259</v>
       </c>
       <c r="J222" t="n">
-        <v>0.30128957545635</v>
+        <v>0.2170203488597468</v>
       </c>
       <c r="K222" t="b">
         <v>0</v>
@@ -9780,7 +9780,7 @@
         <v>8</v>
       </c>
       <c r="C223" t="n">
-        <v>1900</v>
+        <v>1850</v>
       </c>
       <c r="D223" t="n">
         <v>1000</v>
@@ -9793,19 +9793,19 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.70218, 0.975  , 0.66904]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.68578, 0.975  , 0.69614]))</t>
         </is>
       </c>
       <c r="H223" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m804/m804.off</t>
+          <t>testModels/refined_db/8/m802/m802.off</t>
         </is>
       </c>
       <c r="I223" t="n">
-        <v>0.002552374671082288</v>
+        <v>6.509696913035947e-05</v>
       </c>
       <c r="J223" t="n">
-        <v>0.4143275475168</v>
+        <v>0.4212982889336</v>
       </c>
       <c r="K223" t="b">
         <v>0</v>
@@ -9822,10 +9822,10 @@
         <v>8</v>
       </c>
       <c r="C224" t="n">
-        <v>1992</v>
+        <v>2000</v>
       </c>
       <c r="D224" t="n">
-        <v>1000</v>
+        <v>1058</v>
       </c>
       <c r="E224" t="b">
         <v>1</v>
@@ -9835,19 +9835,19 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.72976, 0.975  , 0.72976]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.5701 , 0.975  , 0.60681]))</t>
         </is>
       </c>
       <c r="H224" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m805/m805.off</t>
+          <t>testModels/refined_db/8/m803/m803.off</t>
         </is>
       </c>
       <c r="I224" t="n">
-        <v>0.0003921532034501675</v>
+        <v>0.0001037527882258007</v>
       </c>
       <c r="J224" t="n">
-        <v>0.4718550028118</v>
+        <v>0.30128957545635</v>
       </c>
       <c r="K224" t="b">
         <v>0</v>
@@ -9864,7 +9864,7 @@
         <v>8</v>
       </c>
       <c r="C225" t="n">
-        <v>1968</v>
+        <v>1900</v>
       </c>
       <c r="D225" t="n">
         <v>1000</v>
@@ -9877,19 +9877,19 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.35829, 0.975  , 0.41154]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.70218, 0.975  , 0.66904]))</t>
         </is>
       </c>
       <c r="H225" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m806/m806.off</t>
+          <t>testModels/refined_db/8/m804/m804.off</t>
         </is>
       </c>
       <c r="I225" t="n">
-        <v>6.230126594257498e-05</v>
+        <v>0.002552374671082288</v>
       </c>
       <c r="J225" t="n">
-        <v>0.12238963667975</v>
+        <v>0.4143275475168</v>
       </c>
       <c r="K225" t="b">
         <v>0</v>
@@ -9906,7 +9906,7 @@
         <v>8</v>
       </c>
       <c r="C226" t="n">
-        <v>1976</v>
+        <v>1992</v>
       </c>
       <c r="D226" t="n">
         <v>1000</v>
@@ -9919,19 +9919,19 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.405  , 0.975  , 0.40384]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.72976, 0.975  , 0.72976]))</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m807/m807.off</t>
+          <t>testModels/refined_db/8/m805/m805.off</t>
         </is>
       </c>
       <c r="I226" t="n">
-        <v>0.001213741904721069</v>
+        <v>0.0003921532034501675</v>
       </c>
       <c r="J226" t="n">
-        <v>0.136760518</v>
+        <v>0.4718550028118</v>
       </c>
       <c r="K226" t="b">
         <v>0</v>
@@ -9948,7 +9948,7 @@
         <v>8</v>
       </c>
       <c r="C227" t="n">
-        <v>1660</v>
+        <v>1968</v>
       </c>
       <c r="D227" t="n">
         <v>1000</v>
@@ -9961,19 +9961,19 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.55085, 0.975  , 0.62458]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.35829, 0.975  , 0.41154]))</t>
         </is>
       </c>
       <c r="H227" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m808/m808.off</t>
+          <t>testModels/refined_db/8/m806/m806.off</t>
         </is>
       </c>
       <c r="I227" t="n">
-        <v>0.0005334409098800224</v>
+        <v>6.230126594257498e-05</v>
       </c>
       <c r="J227" t="n">
-        <v>0.29952589509265</v>
+        <v>0.12238963667975</v>
       </c>
       <c r="K227" t="b">
         <v>0</v>
@@ -9990,7 +9990,7 @@
         <v>8</v>
       </c>
       <c r="C228" t="n">
-        <v>1940</v>
+        <v>1976</v>
       </c>
       <c r="D228" t="n">
         <v>1000</v>
@@ -10003,19 +10003,19 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.24254, 0.975  , 0.22572]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.405  , 0.975  , 0.40384]))</t>
         </is>
       </c>
       <c r="H228" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m809/m809.off</t>
+          <t>testModels/refined_db/8/m807/m807.off</t>
         </is>
       </c>
       <c r="I228" t="n">
-        <v>0.001741736583522547</v>
+        <v>0.001213741904721069</v>
       </c>
       <c r="J228" t="n">
-        <v>0.04148136539820001</v>
+        <v>0.136760518</v>
       </c>
       <c r="K228" t="b">
         <v>0</v>
@@ -10032,7 +10032,7 @@
         <v>8</v>
       </c>
       <c r="C229" t="n">
-        <v>1944</v>
+        <v>1660</v>
       </c>
       <c r="D229" t="n">
         <v>1000</v>
@@ -10045,19 +10045,19 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.38296, 0.975  , 0.3995 ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.55085, 0.975  , 0.62458]))</t>
         </is>
       </c>
       <c r="H229" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m810/m810.off</t>
+          <t>testModels/refined_db/8/m808/m808.off</t>
         </is>
       </c>
       <c r="I229" t="n">
-        <v>0.0005863661447857373</v>
+        <v>0.0005334409098800224</v>
       </c>
       <c r="J229" t="n">
-        <v>0.1273507914384</v>
+        <v>0.29952589509265</v>
       </c>
       <c r="K229" t="b">
         <v>0</v>
@@ -10074,10 +10074,10 @@
         <v>8</v>
       </c>
       <c r="C230" t="n">
-        <v>1920</v>
+        <v>1940</v>
       </c>
       <c r="D230" t="n">
-        <v>964</v>
+        <v>1000</v>
       </c>
       <c r="E230" t="b">
         <v>1</v>
@@ -10087,19 +10087,19 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.53825, 0.975  , 0.55673]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.24254, 0.975  , 0.22572]))</t>
         </is>
       </c>
       <c r="H230" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m811/m811.off</t>
+          <t>testModels/refined_db/8/m809/m809.off</t>
         </is>
       </c>
       <c r="I230" t="n">
-        <v>0.0003918203221181705</v>
+        <v>0.001741736583522547</v>
       </c>
       <c r="J230" t="n">
-        <v>0.2592673744301999</v>
+        <v>0.04148136539820001</v>
       </c>
       <c r="K230" t="b">
         <v>0</v>
@@ -10116,10 +10116,10 @@
         <v>8</v>
       </c>
       <c r="C231" t="n">
-        <v>1920</v>
+        <v>1944</v>
       </c>
       <c r="D231" t="n">
-        <v>976</v>
+        <v>1000</v>
       </c>
       <c r="E231" t="b">
         <v>1</v>
@@ -10129,19 +10129,19 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.46015, 0.975  , 0.47582]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.38296, 0.975  , 0.3995 ]))</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
         <is>
-          <t>testModels/refined_db/8/m812/m812.off</t>
+          <t>testModels/refined_db/8/m810/m810.off</t>
         </is>
       </c>
       <c r="I231" t="n">
-        <v>9.637779485730415e-05</v>
+        <v>0.0005863661447857373</v>
       </c>
       <c r="J231" t="n">
-        <v>0.18636813187305</v>
+        <v>0.1273507914384</v>
       </c>
       <c r="K231" t="b">
         <v>0</v>
@@ -10155,13 +10155,13 @@
         <v>230</v>
       </c>
       <c r="B232" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C232" t="n">
-        <v>1772</v>
+        <v>1920</v>
       </c>
       <c r="D232" t="n">
-        <v>1000</v>
+        <v>964</v>
       </c>
       <c r="E232" t="b">
         <v>1</v>
@@ -10171,19 +10171,19 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.61843, 0.38125]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.53825, 0.975  , 0.55673]))</t>
         </is>
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m900/m900.off</t>
+          <t>testModels/refined_db/8/m811/m811.off</t>
         </is>
       </c>
       <c r="I232" t="n">
-        <v>0.0009292084722142014</v>
+        <v>0.0003918203221181705</v>
       </c>
       <c r="J232" t="n">
-        <v>0.2008387393843999</v>
+        <v>0.2592673744301999</v>
       </c>
       <c r="K232" t="b">
         <v>0</v>
@@ -10197,13 +10197,13 @@
         <v>231</v>
       </c>
       <c r="B233" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C233" t="n">
-        <v>1980</v>
+        <v>1920</v>
       </c>
       <c r="D233" t="n">
-        <v>1000</v>
+        <v>976</v>
       </c>
       <c r="E233" t="b">
         <v>1</v>
@@ -10213,19 +10213,19 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.74465, 0.75526]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.46015, 0.975  , 0.47582]))</t>
         </is>
       </c>
       <c r="H233" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m901/m901.off</t>
+          <t>testModels/refined_db/8/m812/m812.off</t>
         </is>
       </c>
       <c r="I233" t="n">
-        <v>0.0008655712038301684</v>
+        <v>9.637779485730415e-05</v>
       </c>
       <c r="J233" t="n">
-        <v>0.4992543045531</v>
+        <v>0.18636813187305</v>
       </c>
       <c r="K233" t="b">
         <v>0</v>
@@ -10242,7 +10242,7 @@
         <v>9</v>
       </c>
       <c r="C234" t="n">
-        <v>1976</v>
+        <v>1772</v>
       </c>
       <c r="D234" t="n">
         <v>1000</v>
@@ -10255,19 +10255,19 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.59618, 0.43685]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.61843, 0.38125]))</t>
         </is>
       </c>
       <c r="H234" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m902/m902.off</t>
+          <t>testModels/refined_db/9/m900/m900.off</t>
         </is>
       </c>
       <c r="I234" t="n">
-        <v>0.002001445678988587</v>
+        <v>0.0009292084722142014</v>
       </c>
       <c r="J234" t="n">
-        <v>0.2234783074855499</v>
+        <v>0.2008387393843999</v>
       </c>
       <c r="K234" t="b">
         <v>0</v>
@@ -10297,19 +10297,19 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.25027, 0.23617]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.74465, 0.75526]))</t>
         </is>
       </c>
       <c r="H235" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m903/m903.off</t>
+          <t>testModels/refined_db/9/m901/m901.off</t>
         </is>
       </c>
       <c r="I235" t="n">
-        <v>0.00108864211424962</v>
+        <v>0.0008655712038301684</v>
       </c>
       <c r="J235" t="n">
-        <v>0.0451911105855</v>
+        <v>0.4992543045531</v>
       </c>
       <c r="K235" t="b">
         <v>0</v>
@@ -10326,7 +10326,7 @@
         <v>9</v>
       </c>
       <c r="C236" t="n">
-        <v>1896</v>
+        <v>1976</v>
       </c>
       <c r="D236" t="n">
         <v>1000</v>
@@ -10339,19 +10339,19 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.40595, 0.975  , 0.40595]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.59618, 0.43685]))</t>
         </is>
       </c>
       <c r="H236" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m904/m904.off</t>
+          <t>testModels/refined_db/9/m902/m902.off</t>
         </is>
       </c>
       <c r="I236" t="n">
-        <v>9.153055386713679e-05</v>
+        <v>0.002001445678988587</v>
       </c>
       <c r="J236" t="n">
-        <v>0.13786748118095</v>
+        <v>0.2234783074855499</v>
       </c>
       <c r="K236" t="b">
         <v>0</v>
@@ -10368,10 +10368,10 @@
         <v>9</v>
       </c>
       <c r="C237" t="n">
-        <v>1972</v>
+        <v>1980</v>
       </c>
       <c r="D237" t="n">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="E237" t="b">
         <v>1</v>
@@ -10381,19 +10381,19 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.84105, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.25027, 0.23617]))</t>
         </is>
       </c>
       <c r="H237" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m905/m905.off</t>
+          <t>testModels/refined_db/9/m903/m903.off</t>
         </is>
       </c>
       <c r="I237" t="n">
-        <v>0.01783165915719444</v>
+        <v>0.00108864211424962</v>
       </c>
       <c r="J237" t="n">
-        <v>0.7364851249999999</v>
+        <v>0.0451911105855</v>
       </c>
       <c r="K237" t="b">
         <v>0</v>
@@ -10410,7 +10410,7 @@
         <v>9</v>
       </c>
       <c r="C238" t="n">
-        <v>1956</v>
+        <v>1896</v>
       </c>
       <c r="D238" t="n">
         <v>1000</v>
@@ -10423,19 +10423,19 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.73251, 0.35051, 0.975  ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.40595, 0.975  , 0.40595]))</t>
         </is>
       </c>
       <c r="H238" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m906/m906.off</t>
+          <t>testModels/refined_db/9/m904/m904.off</t>
         </is>
       </c>
       <c r="I238" t="n">
-        <v>9.369465416477644e-05</v>
+        <v>9.153055386713679e-05</v>
       </c>
       <c r="J238" t="n">
-        <v>0.2187877917004</v>
+        <v>0.13786748118095</v>
       </c>
       <c r="K238" t="b">
         <v>0</v>
@@ -10452,10 +10452,10 @@
         <v>9</v>
       </c>
       <c r="C239" t="n">
-        <v>1898</v>
+        <v>1972</v>
       </c>
       <c r="D239" t="n">
-        <v>1000</v>
+        <v>995</v>
       </c>
       <c r="E239" t="b">
         <v>1</v>
@@ -10465,19 +10465,19 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.46091, 0.975  , 0.46112]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.84105, 0.975  ]))</t>
         </is>
       </c>
       <c r="H239" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m907/m907.off</t>
+          <t>testModels/refined_db/9/m905/m905.off</t>
         </is>
       </c>
       <c r="I239" t="n">
-        <v>9.091806591361756e-08</v>
+        <v>0.01783165915719444</v>
       </c>
       <c r="J239" t="n">
-        <v>0.1806036165228</v>
+        <v>0.7364851249999999</v>
       </c>
       <c r="K239" t="b">
         <v>0</v>
@@ -10494,7 +10494,7 @@
         <v>9</v>
       </c>
       <c r="C240" t="n">
-        <v>1772</v>
+        <v>1956</v>
       </c>
       <c r="D240" t="n">
         <v>1000</v>
@@ -10507,19 +10507,19 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.38093, 0.5    ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.73251, 0.35051, 0.975  ]))</t>
         </is>
       </c>
       <c r="H240" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m908/m908.off</t>
+          <t>testModels/refined_db/9/m906/m906.off</t>
         </is>
       </c>
       <c r="I240" t="n">
-        <v>0.0006813556252919533</v>
+        <v>9.369465416477644e-05</v>
       </c>
       <c r="J240" t="n">
-        <v>0.1606127350113</v>
+        <v>0.2187877917004</v>
       </c>
       <c r="K240" t="b">
         <v>0</v>
@@ -10536,7 +10536,7 @@
         <v>9</v>
       </c>
       <c r="C241" t="n">
-        <v>1974</v>
+        <v>1898</v>
       </c>
       <c r="D241" t="n">
         <v>1000</v>
@@ -10549,19 +10549,19 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.47863, 0.5    ]))</t>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.46091, 0.975  , 0.46112]))</t>
         </is>
       </c>
       <c r="H241" t="inlineStr">
         <is>
-          <t>testModels/refined_db/9/m911/m911.off</t>
+          <t>testModels/refined_db/9/m907/m907.off</t>
         </is>
       </c>
       <c r="I241" t="n">
-        <v>0.004597958658645679</v>
+        <v>9.091806591361756e-08</v>
       </c>
       <c r="J241" t="n">
-        <v>0.20469828125</v>
+        <v>0.1806036165228</v>
       </c>
       <c r="K241" t="b">
         <v>0</v>
@@ -10578,7 +10578,7 @@
         <v>9</v>
       </c>
       <c r="C242" t="n">
-        <v>1988</v>
+        <v>1772</v>
       </c>
       <c r="D242" t="n">
         <v>1000</v>
@@ -10591,24 +10591,150 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.38093, 0.5    ]))</t>
+        </is>
+      </c>
+      <c r="H242" t="inlineStr">
+        <is>
+          <t>testModels/refined_db/9/m908/m908.off</t>
+        </is>
+      </c>
+      <c r="I242" t="n">
+        <v>0.0006813556252919533</v>
+      </c>
+      <c r="J242" t="n">
+        <v>0.1606127350113</v>
+      </c>
+      <c r="K242" t="b">
+        <v>0</v>
+      </c>
+      <c r="L242" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="n">
+        <v>241</v>
+      </c>
+      <c r="B243" t="n">
+        <v>9</v>
+      </c>
+      <c r="C243" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D243" t="n">
+        <v>1010</v>
+      </c>
+      <c r="E243" t="b">
+        <v>1</v>
+      </c>
+      <c r="F243" t="b">
+        <v>0</v>
+      </c>
+      <c r="G243" t="inlineStr">
+        <is>
+          <t>(TrackedArray([0.025  , 0.02623, 0.025  ]), TrackedArray([0.70357, 0.44378, 0.975  ]))</t>
+        </is>
+      </c>
+      <c r="H243" t="inlineStr">
+        <is>
+          <t>testModels/refined_db/9/m909/m909.off</t>
+        </is>
+      </c>
+      <c r="I243" t="n">
+        <v>0.1286547542692651</v>
+      </c>
+      <c r="J243" t="n">
+        <v>0.2691700682120299</v>
+      </c>
+      <c r="K243" t="b">
+        <v>0</v>
+      </c>
+      <c r="L243" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="1" t="n">
+        <v>242</v>
+      </c>
+      <c r="B244" t="n">
+        <v>9</v>
+      </c>
+      <c r="C244" t="n">
+        <v>1974</v>
+      </c>
+      <c r="D244" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E244" t="b">
+        <v>1</v>
+      </c>
+      <c r="F244" t="b">
+        <v>0</v>
+      </c>
+      <c r="G244" t="inlineStr">
+        <is>
+          <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975  , 0.47863, 0.5    ]))</t>
+        </is>
+      </c>
+      <c r="H244" t="inlineStr">
+        <is>
+          <t>testModels/refined_db/9/m911/m911.off</t>
+        </is>
+      </c>
+      <c r="I244" t="n">
+        <v>0.004597958658645679</v>
+      </c>
+      <c r="J244" t="n">
+        <v>0.20469828125</v>
+      </c>
+      <c r="K244" t="b">
+        <v>0</v>
+      </c>
+      <c r="L244" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="1" t="n">
+        <v>243</v>
+      </c>
+      <c r="B245" t="n">
+        <v>9</v>
+      </c>
+      <c r="C245" t="n">
+        <v>1988</v>
+      </c>
+      <c r="D245" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E245" t="b">
+        <v>1</v>
+      </c>
+      <c r="F245" t="b">
+        <v>0</v>
+      </c>
+      <c r="G245" t="inlineStr">
+        <is>
           <t>(TrackedArray([0.025, 0.025, 0.025]), TrackedArray([0.975, 0.5  , 0.5  ]))</t>
         </is>
       </c>
-      <c r="H242" t="inlineStr">
+      <c r="H245" t="inlineStr">
         <is>
           <t>testModels/refined_db/9/m912/m912.off</t>
         </is>
       </c>
-      <c r="I242" t="n">
+      <c r="I245" t="n">
         <v>0.001119938230630489</v>
       </c>
-      <c r="J242" t="n">
+      <c r="J245" t="n">
         <v>0.21434375</v>
       </c>
-      <c r="K242" t="b">
-        <v>0</v>
-      </c>
-      <c r="L242" t="b">
+      <c r="K245" t="b">
+        <v>0</v>
+      </c>
+      <c r="L245" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>